<commit_message>
fix bug that didn't render new bros
</commit_message>
<xml_diff>
--- a/src/data/summer21/bios_summer21.xlsx
+++ b/src/data/summer21/bios_summer21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyenokida/Projects/dspuci-website-gatsby/src/data/summer21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0423544-AEBD-234A-A5CE-AE7DBC04942E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C7D732-9729-6345-B43A-6533FD03519A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31560" yWindow="-2200" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1545,15 +1545,17 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L41" sqref="L41"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="5" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="79.1640625" customWidth="1"/>
+    <col min="3" max="5" width="21.5" customWidth="1"/>
     <col min="6" max="6" width="25.6640625" customWidth="1"/>
     <col min="7" max="7" width="46" customWidth="1"/>
     <col min="8" max="8" width="40.83203125" customWidth="1"/>

</xml_diff>

<commit_message>
fixed issue with bros' minors, updated bios, changed default career year
</commit_message>
<xml_diff>
--- a/src/data/summer21/bios_summer21.xlsx
+++ b/src/data/summer21/bios_summer21.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyenokida/Projects/dspuci-website-gatsby/src/data/summer21/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brennenwong/dspuci-website-gatsby/src/data/summer21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C7D732-9729-6345-B43A-6533FD03519A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B000D86F-B2D9-2E4E-A2FE-A4F14819BF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31560" yWindow="-2200" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="374">
   <si>
     <t>Timestamp</t>
   </si>
@@ -488,9 +488,6 @@
   </si>
   <si>
     <t>Alpha Kappa</t>
-  </si>
-  <si>
-    <t>Literary Journalism, Digital Information Systems</t>
   </si>
   <si>
     <t>Finance, Consulting</t>
@@ -1140,6 +1137,12 @@
   <si>
     <t xml:space="preserve">Hi! My name is Tiffany Than and I initiated in my fall quarter of my first year here at UCI in 2019. In my free time I enjoy exploring new eateries, making Spotify playlists, and seeing live concerts! A fun fact about myself is that I named my car Adeline. Ask me about music/tv shows, my thoughts on mukbangs, or anything at recruitment! 
 </t>
+  </si>
+  <si>
+    <t>Literary Journalism, Information and Computer Science</t>
+  </si>
+  <si>
+    <t>Recruitment + Retention Intern at ASUCI</t>
   </si>
 </sst>
 </file>
@@ -1545,21 +1548,21 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="79.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
     <col min="3" max="5" width="21.5" customWidth="1"/>
     <col min="6" max="6" width="25.6640625" customWidth="1"/>
     <col min="7" max="7" width="46" customWidth="1"/>
     <col min="8" max="8" width="40.83203125" customWidth="1"/>
-    <col min="9" max="9" width="39" customWidth="1"/>
+    <col min="9" max="9" width="45.5" customWidth="1"/>
     <col min="10" max="10" width="83.33203125" customWidth="1"/>
     <col min="11" max="11" width="96.6640625" customWidth="1"/>
     <col min="12" max="12" width="21.5" customWidth="1"/>
@@ -1620,116 +1623,112 @@
     </row>
     <row r="2" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
-        <v>44410.840196759258</v>
+        <v>44396.977627314816</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>152</v>
+        <v>58</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>153</v>
+        <v>59</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>154</v>
+        <v>204</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>155</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>156</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>157</v>
+        <v>205</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>158</v>
+        <v>206</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>159</v>
+        <v>207</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>161</v>
+        <v>62</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>162</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
-        <v>44411.590104166666</v>
+        <v>44404.516250000001</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>222</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>223</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>163</v>
+        <v>224</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>16</v>
+        <v>184</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>29</v>
+        <v>225</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>164</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>165</v>
+        <v>226</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>166</v>
+        <v>227</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>167</v>
+        <v>31</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>143</v>
+        <v>106</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>168</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
-        <v>44409.75885416667</v>
+        <v>44409.634976851848</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>102</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>169</v>
+        <v>338</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -1738,46 +1737,48 @@
         <v>43</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="J4" s="2" t="s">
-        <v>30</v>
+        <v>339</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>170</v>
+        <v>340</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>171</v>
+        <v>341</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>172</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
-        <v>44396.99490740741</v>
+        <v>44404.857893518521</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>173</v>
+        <v>313</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>174</v>
+        <v>314</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>175</v>
+        <v>315</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>155</v>
@@ -1786,96 +1787,94 @@
         <v>17</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>176</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>72</v>
+        <v>316</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>177</v>
+        <v>317</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>178</v>
+        <v>318</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>179</v>
+        <v>319</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>180</v>
+        <v>320</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>181</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
-        <v>44410.762546296297</v>
+        <v>44397.64371527778</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>182</v>
+        <v>64</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>183</v>
+        <v>65</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>184</v>
+        <v>231</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>185</v>
+        <v>49</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>186</v>
+        <v>66</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>187</v>
+        <v>232</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>31</v>
+        <v>233</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>189</v>
+        <v>67</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>190</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
-        <v>44411.033541666664</v>
+        <v>44416.612488425926</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>191</v>
+        <v>322</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>42</v>
@@ -1884,55 +1883,55 @@
         <v>23</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>192</v>
+        <v>323</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>44</v>
+        <v>324</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>193</v>
+        <v>31</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>194</v>
+        <v>20</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>195</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
-        <v>44042.649953703702</v>
+        <v>44404.653217592589</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>358</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>48</v>
+        <v>359</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>196</v>
+        <v>360</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>49</v>
+        <v>184</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>50</v>
+        <v>361</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>51</v>
@@ -1942,45 +1941,45 @@
         <v>52</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>53</v>
+        <v>362</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>54</v>
+        <v>363</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>137</v>
+        <v>67</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>365</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>57</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
-        <v>44397.036516203705</v>
+        <v>44397.382604166669</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>197</v>
+        <v>117</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>198</v>
+        <v>118</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>155</v>
+        <v>42</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>200</v>
+        <v>66</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>51</v>
@@ -1990,84 +1989,86 @@
         <v>52</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N9" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>203</v>
+      <c r="N9" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
-        <v>44396.977627314816</v>
+        <v>44396.99622685185</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>58</v>
+        <v>212</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>155</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>60</v>
+        <v>214</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I10" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>215</v>
+      </c>
       <c r="J10" s="2" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>130</v>
+        <v>26</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
-        <v>44397.382604166669</v>
+        <v>44404.873078703706</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>210</v>
+        <v>267</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>42</v>
@@ -2076,340 +2077,340 @@
         <v>23</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>52</v>
+        <v>268</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>211</v>
+        <v>269</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>31</v>
+        <v>270</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>119</v>
+        <v>39</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>212</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
-        <v>44396.99622685185</v>
+        <v>44396.943645833337</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>213</v>
+        <v>257</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>214</v>
+        <v>258</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>155</v>
+        <v>42</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>215</v>
+        <v>75</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>216</v>
-      </c>
+      <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>217</v>
+        <v>25</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>218</v>
+        <v>259</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>219</v>
+        <v>76</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>222</v>
+        <v>55</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
-        <v>44404.516250000001</v>
+        <v>44042.649953703702</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>223</v>
+        <v>47</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>224</v>
+        <v>48</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>185</v>
+        <v>49</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>226</v>
+        <v>50</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
-        <v>227</v>
+        <v>52</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>228</v>
+        <v>53</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>230</v>
+        <v>55</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>231</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
-        <v>44397.64371527778</v>
+        <v>44398.992349537039</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>64</v>
+        <v>304</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>65</v>
+        <v>305</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>232</v>
+        <v>306</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>49</v>
+        <v>184</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I14" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>307</v>
+      </c>
       <c r="J14" s="2" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>233</v>
+        <v>308</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="O14" s="5" t="s">
-        <v>132</v>
+        <v>193</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>311</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>235</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
-        <v>44409.99291666667</v>
+        <v>44398.099432870367</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>236</v>
+        <v>88</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>237</v>
+        <v>89</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>238</v>
+        <v>295</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>185</v>
+        <v>42</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>239</v>
+        <v>296</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
-        <v>240</v>
+        <v>90</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>31</v>
+        <v>297</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>31</v>
+        <v>298</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>242</v>
+        <v>91</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>138</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>243</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
-        <v>44397.883923611109</v>
+        <v>44404.807638888888</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>244</v>
+        <v>94</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>245</v>
+        <v>300</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>185</v>
+        <v>16</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>246</v>
+        <v>104</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>247</v>
+        <v>30</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>248</v>
+        <v>301</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>249</v>
+        <v>302</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>251</v>
+        <v>67</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>252</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
-        <v>44399.908993055556</v>
+        <v>44046.843055555553</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>69</v>
+        <v>120</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>70</v>
+        <v>121</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>253</v>
+        <v>326</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>18</v>
+        <v>122</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>71</v>
+        <v>327</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>254</v>
+        <v>25</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>255</v>
+        <v>123</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>256</v>
+        <v>124</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>73</v>
+        <v>125</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>257</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
-        <v>44396.943645833337</v>
+        <v>44410.679201388892</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>258</v>
+        <v>78</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>42</v>
@@ -2418,288 +2419,292 @@
         <v>23</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>75</v>
+        <v>262</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>76</v>
+        <v>265</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>55</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="P18" s="6" t="s">
-        <v>261</v>
+        <v>141</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
-        <v>44410.679201388892</v>
+        <v>44410.762546296297</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>78</v>
+        <v>181</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>79</v>
+        <v>182</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>262</v>
+        <v>183</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>42</v>
+        <v>184</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>263</v>
+        <v>185</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
-        <v>264</v>
+        <v>30</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>265</v>
+        <v>186</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>266</v>
+        <v>31</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="O19" s="5" t="s">
-        <v>141</v>
+        <v>20</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>267</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
-        <v>44404.873078703706</v>
+        <v>44409.75885416667</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>268</v>
+        <v>168</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>269</v>
+        <v>30</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>270</v>
+        <v>169</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>271</v>
+        <v>170</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>272</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
-        <v>44411.616377314815</v>
+        <v>44396.99490740741</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>82</v>
+        <v>172</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>85</v>
+        <v>173</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>273</v>
+        <v>174</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>16</v>
+        <v>155</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>86</v>
+        <v>175</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>274</v>
+        <v>72</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>275</v>
+        <v>176</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>276</v>
+        <v>177</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="O21" s="5" t="s">
-        <v>147</v>
+        <v>26</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>277</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
-        <v>44411.776064814818</v>
+        <v>44397.883923611109</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>278</v>
+        <v>69</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>281</v>
+        <v>18</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I22" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>245</v>
+      </c>
       <c r="J22" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>31</v>
+        <v>247</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>194</v>
+        <v>26</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>283</v>
+        <v>249</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>284</v>
+        <v>250</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>285</v>
+        <v>251</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
-        <v>44396.946180555555</v>
+        <v>44411.590104166666</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>286</v>
+        <v>14</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>287</v>
+        <v>15</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>288</v>
+        <v>162</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>155</v>
+        <v>16</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="I23" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="J23" s="2" t="s">
-        <v>290</v>
+        <v>164</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>291</v>
+        <v>165</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>292</v>
+        <v>166</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N23" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>294</v>
+        <v>20</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>143</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>295</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
-        <v>44398.099432870367</v>
+        <v>44411.026041666664</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>296</v>
+        <v>343</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>42</v>
@@ -2711,617 +2716,615 @@
         <v>38</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>297</v>
+        <v>24</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2" t="s">
-        <v>90</v>
+        <v>344</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>298</v>
+        <v>345</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>299</v>
+        <v>346</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>300</v>
+        <v>347</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
-        <v>44404.807638888888</v>
+        <v>44399.908993055556</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>301</v>
+        <v>252</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>95</v>
+        <v>18</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>30</v>
+        <v>253</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>302</v>
+        <v>254</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>303</v>
+        <v>255</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>96</v>
+        <v>36</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>304</v>
+        <v>256</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
-        <v>44398.992349537039</v>
+        <v>44409.99291666667</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>305</v>
+        <v>235</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>306</v>
+        <v>236</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>307</v>
+        <v>237</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="3">
+        <v>44397.626064814816</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="N26" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A27" s="3">
-        <v>44404.857893518521</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="G27" s="2" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I27" s="2"/>
+      <c r="I27" s="2" t="s">
+        <v>368</v>
+      </c>
       <c r="J27" s="2" t="s">
-        <v>317</v>
+        <v>90</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>318</v>
+        <v>369</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>319</v>
+        <v>370</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N27" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="O27" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>322</v>
+        <v>26</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="O27" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="P27" s="8" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
-        <v>44416.612488425926</v>
+        <v>44411.616377314815</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>323</v>
+        <v>272</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>99</v>
+        <v>29</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I28" s="2"/>
+      <c r="I28" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="J28" s="2" t="s">
-        <v>324</v>
+        <v>273</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>325</v>
+        <v>274</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>31</v>
+        <v>275</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>326</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
-        <v>44046.843055555553</v>
+        <v>44413.04755787037</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>327</v>
+        <v>353</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>328</v>
-      </c>
+      <c r="I29" s="2"/>
       <c r="J29" s="2" t="s">
-        <v>25</v>
+        <v>354</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>123</v>
+        <v>355</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>124</v>
+        <v>356</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N29" s="5" t="s">
-        <v>125</v>
+        <v>91</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>126</v>
+        <v>357</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
-        <v>44405.648368055554</v>
+        <v>44396.959282407406</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>329</v>
+        <v>110</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>330</v>
+        <v>37</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>331</v>
+        <v>348</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>155</v>
+        <v>16</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>332</v>
+        <v>349</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>216</v>
-      </c>
+      <c r="I30" s="2"/>
       <c r="J30" s="2" t="s">
-        <v>333</v>
+        <v>25</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>334</v>
+        <v>350</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>335</v>
+        <v>351</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N30" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="O30" s="2" t="s">
-        <v>337</v>
+        <v>26</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="O30" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>338</v>
+        <v>352</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
-        <v>44409.634976851848</v>
+        <v>44410.840196759258</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>101</v>
+        <v>152</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>339</v>
+        <v>154</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>16</v>
+        <v>155</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>104</v>
+        <v>372</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>340</v>
+        <v>156</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>341</v>
+        <v>157</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>342</v>
+        <v>158</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N31" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="O31" s="5" t="s">
-        <v>131</v>
+        <v>106</v>
+      </c>
+      <c r="N31" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>343</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
-        <v>44411.026041666664</v>
+        <v>44397.036516203705</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>108</v>
+        <v>196</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>15</v>
+        <v>197</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>344</v>
+        <v>198</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>42</v>
+        <v>155</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>38</v>
+        <v>199</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2" t="s">
-        <v>345</v>
+        <v>52</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>346</v>
+        <v>200</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>347</v>
+        <v>45</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="O32" s="5" t="s">
-        <v>144</v>
+        <v>26</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>202</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>348</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
-        <v>44396.959282407406</v>
+        <v>44411.776064814818</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>110</v>
+        <v>277</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>37</v>
+        <v>278</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>349</v>
+        <v>279</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>16</v>
+        <v>184</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>350</v>
+        <v>280</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2" t="s">
-        <v>25</v>
+        <v>281</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>351</v>
+        <v>373</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>352</v>
+        <v>45</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="O33" s="5" t="s">
-        <v>149</v>
+        <v>193</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="O33" s="2" t="s">
+        <v>283</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>353</v>
+        <v>284</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
-        <v>44413.04755787037</v>
+        <v>44405.648368055554</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>113</v>
+        <v>328</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>127</v>
+        <v>329</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>16</v>
+        <v>155</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>95</v>
+        <v>331</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I34" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>215</v>
+      </c>
       <c r="J34" s="2" t="s">
-        <v>355</v>
+        <v>332</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>356</v>
+        <v>333</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>357</v>
+        <v>334</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="N34" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="O34" s="5" t="s">
-        <v>148</v>
+        <v>55</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>336</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>358</v>
+        <v>337</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
-        <v>44404.653217592589</v>
+        <v>44396.946180555555</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>359</v>
+        <v>285</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>360</v>
+        <v>286</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>361</v>
+        <v>287</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>362</v>
+        <v>38</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>51</v>
+        <v>288</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2" t="s">
-        <v>52</v>
+        <v>289</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>363</v>
+        <v>290</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>364</v>
+        <v>291</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>365</v>
+        <v>292</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>366</v>
+        <v>293</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>367</v>
+        <v>294</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
-        <v>44397.626064814816</v>
+        <v>44411.033541666664</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>114</v>
+        <v>40</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>115</v>
+        <v>41</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>368</v>
+        <v>190</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I36" s="2" t="s">
-        <v>369</v>
-      </c>
+      <c r="I36" s="2"/>
       <c r="J36" s="2" t="s">
-        <v>90</v>
+        <v>191</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>370</v>
+        <v>44</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>371</v>
+        <v>192</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>26</v>
+        <v>193</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>116</v>
+        <v>46</v>
       </c>
       <c r="O36" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="P36" s="8" t="s">
-        <v>372</v>
+        <v>150</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3334,6 +3337,9 @@
       <c r="P39" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P39">
+    <sortCondition ref="C2:C39"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reformatted recruitment info and updated bros info
</commit_message>
<xml_diff>
--- a/src/data/summer21/bios_summer21.xlsx
+++ b/src/data/summer21/bios_summer21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brennenwong/Documents/DSP Website/src/data/summer21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4FAE57-4F0C-7E4A-85FD-C1D495282478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A9CE25-B0B9-D447-907A-B9AE1096280A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -583,9 +583,6 @@
     <t>ashley_yeh</t>
   </si>
   <si>
-    <t>UI/UX Design</t>
-  </si>
-  <si>
     <t>Product Association at UCI</t>
   </si>
   <si>
@@ -724,12 +721,6 @@
     <t>dylan_tanzil</t>
   </si>
   <si>
-    <t>Undeclared</t>
-  </si>
-  <si>
-    <t>Product Management, Consulting</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/dylantanzil/</t>
   </si>
   <si>
@@ -797,18 +788,6 @@
   </si>
   <si>
     <t>Saratoga, CA</t>
-  </si>
-  <si>
-    <t>Data Science, Product Management, Security</t>
-  </si>
-  <si>
-    <t>Cyber Risk Intern at Deloitte</t>
-  </si>
-  <si>
-    <t>Sports Statistics Club</t>
-  </si>
-  <si>
-    <t>My name is Gaurav Mohan and I joined DSP in my freshman year as part of the alpha eta class. I am an easy going individual with a strong passion for applying new technology and leveraging data to solve problems within the healthcare, sports, and tech industry. I love to surf, play basketball, workout, and hang out with friends in my free time. Ask my about any of the aforementioned topics at recruitment.</t>
   </si>
   <si>
     <t>grace_hsiang</t>
@@ -1196,7 +1175,28 @@
     <t>Investment Analyst Intern at Interlink Global Investments</t>
   </si>
   <si>
-    <t>Graphic Design Intern at Ingram Micro</t>
+    <t>Product Design</t>
+  </si>
+  <si>
+    <t>UI/UX Designer at Activism Always</t>
+  </si>
+  <si>
+    <t>Data Science, Security, Consulting, PM</t>
+  </si>
+  <si>
+    <t>Cyber Risk Analyst at Deloitte</t>
+  </si>
+  <si>
+    <t>Campus Research @ UCI Stats (Basketball Analytics)</t>
+  </si>
+  <si>
+    <t>My name is Gaurav Mohan and I am a fourth year and joined Pi Sigma as a freshman as part of the Alpha Eta class. I enjoy playing sports (basketball, surfing, tennis, golf), going to concerts, cooking, and traveling. I enjoy sports analytics, investing in crypto, and exploring new areas of tech. Ask me about my trip to Oregon.</t>
+  </si>
+  <si>
+    <t>Consulting, Sales, Marketing</t>
+  </si>
+  <si>
+    <t>Sales Partner at UpMerch</t>
   </si>
 </sst>
 </file>
@@ -1601,11 +1601,11 @@
   </sheetPr>
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="183" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1686,7 +1686,7 @@
         <v>57</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>16</v>
@@ -1702,13 +1702,13 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>60</v>
@@ -1720,7 +1720,7 @@
         <v>127</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1728,13 +1728,13 @@
         <v>44404.516250000001</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>181</v>
@@ -1743,17 +1743,17 @@
         <v>17</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>35</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>31</v>
@@ -1762,13 +1762,13 @@
         <v>104</v>
       </c>
       <c r="N3" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1782,7 +1782,7 @@
         <v>100</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -1800,13 +1800,13 @@
         <v>102</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>60</v>
@@ -1818,7 +1818,7 @@
         <v>128</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1826,13 +1826,13 @@
         <v>44404.857893518521</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>152</v>
@@ -1848,25 +1848,25 @@
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1880,7 +1880,7 @@
         <v>63</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>48</v>
@@ -1899,10 +1899,10 @@
         <v>51</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>229</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>65</v>
@@ -1914,7 +1914,7 @@
         <v>129</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1928,7 +1928,7 @@
         <v>96</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>42</v>
@@ -1944,10 +1944,10 @@
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>31</v>
@@ -1962,7 +1962,7 @@
         <v>130</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -1970,13 +1970,13 @@
         <v>44404.653217592589</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>181</v>
@@ -1985,7 +1985,7 @@
         <v>17</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>50</v>
@@ -1995,22 +1995,22 @@
         <v>51</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>65</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2024,7 +2024,7 @@
         <v>116</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>42</v>
@@ -2043,7 +2043,7 @@
         <v>51</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>31</v>
@@ -2058,7 +2058,7 @@
         <v>131</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2066,13 +2066,13 @@
         <v>44396.99622685185</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>152</v>
@@ -2081,34 +2081,34 @@
         <v>43</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I10" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>214</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N10" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="O10" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2116,13 +2116,13 @@
         <v>44397.802523148152</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>152</v>
@@ -2138,10 +2138,10 @@
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>31</v>
@@ -2150,13 +2150,13 @@
         <v>89</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2170,7 +2170,7 @@
         <v>81</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>42</v>
@@ -2186,13 +2186,13 @@
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>39</v>
@@ -2204,7 +2204,7 @@
         <v>132</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2212,13 +2212,13 @@
         <v>44396.943645833337</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>42</v>
@@ -2237,7 +2237,7 @@
         <v>25</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>74</v>
@@ -2252,7 +2252,7 @@
         <v>133</v>
       </c>
       <c r="P13" s="6" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2266,7 +2266,7 @@
         <v>47</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>48</v>
@@ -2285,7 +2285,7 @@
         <v>51</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>52</v>
@@ -2308,13 +2308,13 @@
         <v>44398.992349537039</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>181</v>
@@ -2329,28 +2329,28 @@
         <v>35</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2364,7 +2364,7 @@
         <v>87</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>42</v>
@@ -2376,17 +2376,17 @@
         <v>38</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>89</v>
@@ -2398,7 +2398,7 @@
         <v>135</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2412,7 +2412,7 @@
         <v>92</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>16</v>
@@ -2433,10 +2433,10 @@
         <v>30</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>65</v>
@@ -2448,7 +2448,7 @@
         <v>136</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2462,7 +2462,7 @@
         <v>119</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>48</v>
@@ -2477,13 +2477,13 @@
         <v>24</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>121</v>
@@ -2512,7 +2512,7 @@
         <v>77</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>42</v>
@@ -2521,20 +2521,20 @@
         <v>23</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>78</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
-        <v>259</v>
+        <v>386</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>260</v>
+        <v>387</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>261</v>
+        <v>388</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>53</v>
@@ -2546,7 +2546,7 @@
         <v>138</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>262</v>
+        <v>389</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2579,7 +2579,7 @@
         <v>30</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>31</v>
@@ -2703,10 +2703,10 @@
         <v>67</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>181</v>
@@ -2721,28 +2721,28 @@
         <v>35</v>
       </c>
       <c r="I23" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="L23" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>244</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2806,7 +2806,7 @@
         <v>15</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>42</v>
@@ -2822,13 +2822,13 @@
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>53</v>
@@ -2840,7 +2840,7 @@
         <v>141</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2854,7 +2854,7 @@
         <v>68</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>48</v>
@@ -2872,13 +2872,13 @@
         <v>69</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>36</v>
@@ -2890,7 +2890,7 @@
         <v>142</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -2898,13 +2898,13 @@
         <v>44409.99291666667</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>233</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>181</v>
@@ -2916,14 +2916,14 @@
         <v>109</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>234</v>
+        <v>35</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2" t="s">
-        <v>235</v>
+        <v>390</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>31</v>
+        <v>391</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>31</v>
@@ -2932,13 +2932,13 @@
         <v>104</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -2952,7 +2952,7 @@
         <v>113</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>16</v>
@@ -2967,16 +2967,16 @@
         <v>24</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>26</v>
@@ -2988,7 +2988,7 @@
         <v>143</v>
       </c>
       <c r="P28" s="8" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -3002,7 +3002,7 @@
         <v>83</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>16</v>
@@ -3020,13 +3020,13 @@
         <v>84</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>53</v>
@@ -3038,7 +3038,7 @@
         <v>144</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -3052,7 +3052,7 @@
         <v>124</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>16</v>
@@ -3068,13 +3068,13 @@
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>89</v>
@@ -3086,7 +3086,7 @@
         <v>145</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -3094,13 +3094,13 @@
         <v>44404.80846064815</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>181</v>
@@ -3109,19 +3109,19 @@
         <v>43</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>31</v>
@@ -3130,13 +3130,13 @@
         <v>36</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -3150,7 +3150,7 @@
         <v>37</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>16</v>
@@ -3159,7 +3159,7 @@
         <v>43</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>35</v>
@@ -3169,10 +3169,10 @@
         <v>25</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>26</v>
@@ -3184,7 +3184,7 @@
         <v>146</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="13" x14ac:dyDescent="0.15">
@@ -3213,7 +3213,7 @@
         <v>24</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>153</v>
@@ -3242,13 +3242,13 @@
         <v>44397.036516203705</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>194</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>152</v>
@@ -3257,7 +3257,7 @@
         <v>17</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>50</v>
@@ -3267,7 +3267,7 @@
         <v>51</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>44</v>
@@ -3276,13 +3276,13 @@
         <v>26</v>
       </c>
       <c r="N34" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="O34" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="O34" s="2" t="s">
+      <c r="P34" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="P34" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3290,13 +3290,13 @@
         <v>44411.776064814818</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>181</v>
@@ -3305,32 +3305,32 @@
         <v>17</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>44</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3338,13 +3338,13 @@
         <v>44405.648368055554</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>152</v>
@@ -3353,34 +3353,34 @@
         <v>17</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>35</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>53</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3388,13 +3388,13 @@
         <v>44396.946180555555</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>152</v>
@@ -3406,29 +3406,29 @@
         <v>38</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="M37" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3458,16 +3458,16 @@
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="L38" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="K38" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="L38" s="2" t="s">
+      <c r="M38" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="N38" s="1" t="s">
         <v>45</v>
@@ -3476,7 +3476,7 @@
         <v>147</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
added new bros and updated chapter stats
</commit_message>
<xml_diff>
--- a/src/data/summer21/bios_summer21.xlsx
+++ b/src/data/summer21/bios_summer21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brennenwong/Documents/DSP Website/src/data/summer21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8FBEFE-DB2B-E54E-9142-1109C57D067D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17CD382-DEAC-3641-91FE-77D8F6D8B1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="500" windowWidth="26960" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="472">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1197,13 +1197,253 @@
   </si>
   <si>
     <t>HR Business Partner, Global Online Intern at The Estee Lauder Companies</t>
+  </si>
+  <si>
+    <t>Nathan</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>nathan_lee</t>
+  </si>
+  <si>
+    <t>Alpha Mu</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>Davis, CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business Administration </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consulting, Finance, Marketing, Real Estate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi! My name is Nathan Lee and I initiated with the Alpha Mu class. I enjoy watching basketball and football and I like thrifting in my free time. My favorite song is Holy Ground by Taylor Swift and you should ask me about my cross country trip at recruitment! </t>
+  </si>
+  <si>
+    <t>nathanlee@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Suman</t>
+  </si>
+  <si>
+    <t>Gujju</t>
+  </si>
+  <si>
+    <t>suman_gujju</t>
+  </si>
+  <si>
+    <t>Consulting, Investing</t>
+  </si>
+  <si>
+    <t>Risk and Financial Advisory Intern at Deloitte</t>
+  </si>
+  <si>
+    <t>Dragon Boat Race Team</t>
+  </si>
+  <si>
+    <t>sumangujju@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Hellooo everyone my name is Suman and I’m a 3rd year Business Economics major who initiated this past Fall with the Alpha Mu class. In my free time I love to play/watch sports and wonder about the existence of aliens. Ask me about my addiction to fantasy football or anything else at recruitment!</t>
+  </si>
+  <si>
+    <t>Forest</t>
+  </si>
+  <si>
+    <t>Huang</t>
+  </si>
+  <si>
+    <t>forest_huang</t>
+  </si>
+  <si>
+    <t>Basking Ridge, NJ</t>
+  </si>
+  <si>
+    <t>Investment Banking, Finance, Esports</t>
+  </si>
+  <si>
+    <t>foresthuang@ucidsp.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi! I’m Forest Huang and I initiated fall of my freshman year as part of the Alpha Mu class. My favorite pastimes include hanging out with friends, trying new foods/restaurants, and playing/watching Esports. A fun fact about me is that I’ve been to two three Michelin starred restaurants (technically 3 if you count takeout). Ask me about video games, stocks, or anything else during recruitment! </t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Lin</t>
+  </si>
+  <si>
+    <t>julia_lin</t>
+  </si>
+  <si>
+    <t>Portland, OR</t>
+  </si>
+  <si>
+    <t>Consulting, Real Estate, Human Resources</t>
+  </si>
+  <si>
+    <t>Youth Vote Intern at Next Up Oregon</t>
+  </si>
+  <si>
+    <t>MUSA Representatives</t>
+  </si>
+  <si>
+    <t>julialin@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Hi hi hi! My name is Julia Lin and I initiated in the fall quarter of my Freshman year with the Alpha Mu class. In my free time, I like to read, travel, and find new shows/movies to watch. Some fun facts about me are that I have my own Lululemon e-commerce business, I've never had a marshmallow before, and I'm also a Canadian Dual-Citizen! Feel free to ask me about anything at recruitment whether it's about the favorite places I've traveled to or about my dog Princess :-)</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Doan</t>
+  </si>
+  <si>
+    <t>andrew_doan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer Science </t>
+  </si>
+  <si>
+    <t>Recruitment and Retention Intern at ASUCI</t>
+  </si>
+  <si>
+    <t>andrewdoan@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Hey there! I'm Andrew, and I initiated in Fall 2021 with the Alpha Mus. I love dance, poetry, traveling, film cameras, hiking, playing sports with friends, and the Notion productivity app. Ask me about art, travel, or anything that impassions you at recruitment; looking forward to meeting you!</t>
+  </si>
+  <si>
+    <t>Jake</t>
+  </si>
+  <si>
+    <t>Moss</t>
+  </si>
+  <si>
+    <t>jake_moss</t>
+  </si>
+  <si>
+    <t>Real Estate Finance, Product Management</t>
+  </si>
+  <si>
+    <t>MUSA</t>
+  </si>
+  <si>
+    <t>jakemoss@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Hi!! My name is Jake and I initiated in the fall of my freshman year with the Alpha Mu class. In my free time, I enjoy surfing, fishing, golfing, playing tennis, and listening to music. A fun fact about myself is that I accidentally lit my couch on fire. Ask me about my favorite comedians, Netflix/tv shows, or anything at recruitment!</t>
+  </si>
+  <si>
+    <t>Jason</t>
+  </si>
+  <si>
+    <t>Henkel</t>
+  </si>
+  <si>
+    <t>jason_henkel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Davis, CA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venture Capital, Entrepreneurship </t>
+  </si>
+  <si>
+    <t>jasonhenkel@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Hi! My name is Jason Henkel and I initiated during the fall of my first year with the Alpha Mu class. Outside of school, I love playing sports, trying new things, and exploring new areas. Ask me about my NBA predictions or favorite movies at recruitment!</t>
+  </si>
+  <si>
+    <t>Elin</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>elin_min</t>
+  </si>
+  <si>
+    <t>Seoul, South Korea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In The Green </t>
+  </si>
+  <si>
+    <t>Hey! My name is Elin Min, and I initiated in Fall 2021 with the Alpha Mu Class. In my free time, I enjoy playing tennis and basketball, working out, and watching crime documentaries. Feel free to ask me about my life in Thailand, Canada, and Korea at recruitment!</t>
+  </si>
+  <si>
+    <t>elinmin@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Winnie</t>
+  </si>
+  <si>
+    <t>Qi</t>
+  </si>
+  <si>
+    <t>winnie_qi</t>
+  </si>
+  <si>
+    <t>San Francisco, CA</t>
+  </si>
+  <si>
+    <t>Finance, Consulting, Product Management</t>
+  </si>
+  <si>
+    <t>Launch@Apple Mentee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Association, Previous: MUSA Representatives, AMP </t>
+  </si>
+  <si>
+    <t>winnieqi@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Hello!!! My name is Winnie and I initiated fall quarter of my second year with the Alpha Mu class. In my free time, I like to play basketball, curate Spotify playlists, and try new food spots. A fun fact about me is that I grew 5 inches in a span of one summer. Ask me about my favorite TV shows, artists, food cuisines, or anything at recruitment :))</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/nathan-lee1/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/julia-lin-2003/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/foresthuang/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/jasonfhenkel/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/suman-gujju/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/andrew-g-doan/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/elin-eunkee-min/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/jakesmoss/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/winnie-qi21/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1249,6 +1489,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1267,10 +1514,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1282,8 +1530,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1599,13 +1850,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P41"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K26" sqref="K26"/>
+      <selection pane="bottomRight" activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1620,8 +1871,8 @@
     <col min="10" max="10" width="83.33203125" customWidth="1"/>
     <col min="11" max="11" width="96.6640625" customWidth="1"/>
     <col min="12" max="12" width="21.5" customWidth="1"/>
-    <col min="13" max="13" width="43.5" customWidth="1"/>
-    <col min="14" max="14" width="21.5" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="24.1640625" customWidth="1"/>
+    <col min="14" max="14" width="36.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="23" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2014,455 +2265,438 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A9" s="3">
-        <v>44397.382604166669</v>
-      </c>
       <c r="B9" s="2" t="s">
-        <v>115</v>
+        <v>426</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>116</v>
+        <v>427</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>203</v>
+        <v>428</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>42</v>
+        <v>395</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>23</v>
+        <v>396</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>64</v>
+        <v>363</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="2"/>
+        <v>429</v>
+      </c>
       <c r="J9" s="2" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>204</v>
+        <v>430</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>131</v>
+        <v>20</v>
+      </c>
+      <c r="N9" t="s">
+        <v>468</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>431</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>205</v>
+        <v>432</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
-        <v>44396.99622685185</v>
+        <v>44397.382604166669</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>206</v>
+        <v>115</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>116</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>152</v>
+        <v>42</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>208</v>
+        <v>64</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>209</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>210</v>
+        <v>51</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>212</v>
+        <v>31</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N10" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>214</v>
+      <c r="N10" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A11" s="3">
-        <v>44397.802523148152</v>
-      </c>
       <c r="B11" s="2" t="s">
-        <v>371</v>
+        <v>402</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>403</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>372</v>
+        <v>404</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>152</v>
+        <v>395</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="J11" s="2" t="s">
-        <v>373</v>
+        <v>405</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>390</v>
+        <v>406</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>31</v>
+        <v>407</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>375</v>
+        <v>53</v>
+      </c>
+      <c r="N11" t="s">
+        <v>467</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>408</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>376</v>
+        <v>409</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
-        <v>44404.873078703706</v>
+        <v>44396.99622685185</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>80</v>
+        <v>206</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>255</v>
+        <v>207</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>42</v>
+        <v>152</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>38</v>
+        <v>208</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>209</v>
+      </c>
       <c r="J12" s="2" t="s">
-        <v>256</v>
+        <v>210</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>257</v>
+        <v>211</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>258</v>
+        <v>212</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>132</v>
+        <v>26</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>388</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
-        <v>44396.943645833337</v>
+        <v>44397.802523148152</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>249</v>
+        <v>371</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>250</v>
+        <v>372</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>42</v>
+        <v>152</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
-        <v>25</v>
+        <v>373</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>251</v>
+        <v>390</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>252</v>
+        <v>89</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A14" s="3">
-        <v>44042.649953703702</v>
-      </c>
       <c r="B14" s="2" t="s">
-        <v>46</v>
+        <v>440</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>47</v>
+        <v>441</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>189</v>
+        <v>442</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>48</v>
+        <v>395</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>43</v>
+        <v>396</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>49</v>
+        <v>443</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" s="2"/>
+        <v>24</v>
+      </c>
       <c r="J14" s="2" t="s">
-        <v>51</v>
+        <v>444</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>378</v>
+        <v>31</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="O14" s="5" t="s">
-        <v>134</v>
+        <v>20</v>
+      </c>
+      <c r="N14" t="s">
+        <v>466</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>445</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>55</v>
+        <v>446</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
-        <v>44398.992349537039</v>
+        <v>44404.873078703706</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>291</v>
+        <v>80</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>292</v>
+        <v>81</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>181</v>
+        <v>42</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>294</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
-        <v>30</v>
+        <v>256</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>295</v>
+        <v>257</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>296</v>
+        <v>258</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>298</v>
+        <v>39</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>299</v>
+        <v>388</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A16" s="3">
-        <v>44398.099432870367</v>
-      </c>
       <c r="B16" s="2" t="s">
-        <v>86</v>
+        <v>410</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>87</v>
+        <v>411</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>282</v>
+        <v>412</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>42</v>
+        <v>395</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>23</v>
+        <v>396</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>38</v>
+        <v>413</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="I16" s="2"/>
+        <v>24</v>
+      </c>
       <c r="J16" s="2" t="s">
-        <v>88</v>
+        <v>414</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>284</v>
+        <v>31</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>285</v>
+        <v>423</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O16" s="5" t="s">
-        <v>135</v>
+        <v>65</v>
+      </c>
+      <c r="N16" t="s">
+        <v>465</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>415</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>286</v>
+        <v>416</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
-        <v>44404.807638888888</v>
+        <v>44396.943645833337</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>91</v>
+        <v>249</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>287</v>
+        <v>250</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>102</v>
-      </c>
+      <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>289</v>
+        <v>251</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>290</v>
+        <v>133</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
-        <v>44046.843055555553</v>
+        <v>44042.649953703702</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>118</v>
+        <v>46</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>119</v>
+        <v>47</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>313</v>
+        <v>189</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>48</v>
@@ -2471,538 +2705,516 @@
         <v>43</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>120</v>
+        <v>49</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>314</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="I18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>121</v>
+        <v>52</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N18" s="5" t="s">
-        <v>122</v>
+      <c r="N18" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>123</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
-        <v>44410.679201388892</v>
+        <v>44398.992349537039</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>76</v>
+        <v>291</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>77</v>
+        <v>292</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>253</v>
+        <v>293</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>42</v>
+        <v>181</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>254</v>
+        <v>105</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="I19" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>294</v>
+      </c>
       <c r="J19" s="2" t="s">
-        <v>382</v>
+        <v>30</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>383</v>
+        <v>295</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>384</v>
+        <v>296</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="O19" s="5" t="s">
-        <v>138</v>
+        <v>187</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>298</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>385</v>
+        <v>299</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
-        <v>44410.762546296297</v>
+        <v>44398.099432870367</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>178</v>
+        <v>86</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>179</v>
+        <v>87</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>180</v>
+        <v>282</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>181</v>
+        <v>42</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>182</v>
+        <v>38</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>35</v>
+        <v>283</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>377</v>
+        <v>284</v>
       </c>
       <c r="L20" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="3">
-        <v>44409.75885416667</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="2" t="s">
+      <c r="L21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N21" t="s">
+        <v>463</v>
+      </c>
+      <c r="O21" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="B22" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O21" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A22" s="3">
-        <v>44396.99490740741</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="J22" s="2" t="s">
-        <v>70</v>
+        <v>421</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>173</v>
+        <v>422</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>174</v>
+        <v>423</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>176</v>
+        <v>53</v>
+      </c>
+      <c r="N22" t="s">
+        <v>464</v>
+      </c>
+      <c r="O22" s="9" t="s">
+        <v>424</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>177</v>
+        <v>425</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
-        <v>44397.883923611109</v>
+        <v>44404.807638888888</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>235</v>
+        <v>92</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>236</v>
+        <v>287</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>181</v>
+        <v>16</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>237</v>
+        <v>102</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>238</v>
+        <v>30</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>239</v>
+        <v>288</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>240</v>
+        <v>289</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N23" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>242</v>
+        <v>65</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>243</v>
+        <v>290</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
-        <v>44411.590104166666</v>
+        <v>44046.843055555553</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>14</v>
+        <v>118</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>159</v>
+        <v>313</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>29</v>
+        <v>120</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>160</v>
+        <v>314</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>161</v>
+        <v>25</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>162</v>
+        <v>379</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>163</v>
+        <v>121</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>21</v>
+        <v>53</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>164</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A25" s="3">
-        <v>44411.026041666664</v>
-      </c>
       <c r="B25" s="2" t="s">
-        <v>106</v>
+        <v>447</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>15</v>
+        <v>448</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>330</v>
+        <v>449</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>42</v>
+        <v>395</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>23</v>
+        <v>396</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>38</v>
+        <v>450</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I25" s="2"/>
+        <v>35</v>
+      </c>
       <c r="J25" s="2" t="s">
-        <v>331</v>
+        <v>220</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>332</v>
+        <v>31</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>333</v>
+        <v>451</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="O25" s="5" t="s">
-        <v>141</v>
+        <v>89</v>
+      </c>
+      <c r="N25" t="s">
+        <v>469</v>
+      </c>
+      <c r="O25" s="9" t="s">
+        <v>453</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>334</v>
+        <v>452</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
-        <v>44399.908993055556</v>
+        <v>44410.679201388892</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>18</v>
+        <v>254</v>
       </c>
       <c r="H26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="B27" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N26" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="O26" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A27" s="3">
-        <v>44409.99291666667</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I27" s="2"/>
       <c r="J27" s="2" t="s">
-        <v>386</v>
+        <v>436</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>387</v>
+        <v>31</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>31</v>
+        <v>437</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N27" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="O27" s="2" t="s">
-        <v>233</v>
+        <v>32</v>
+      </c>
+      <c r="N27" t="s">
+        <v>470</v>
+      </c>
+      <c r="O27" s="9" t="s">
+        <v>438</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>234</v>
+        <v>439</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
-        <v>44397.626064814816</v>
+        <v>44410.762546296297</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>112</v>
+        <v>178</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>113</v>
+        <v>179</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>354</v>
+        <v>180</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>16</v>
+        <v>181</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>49</v>
+        <v>182</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>355</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="I28" s="2"/>
       <c r="J28" s="2" t="s">
-        <v>88</v>
+        <v>30</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>356</v>
+        <v>31</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="O28" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="P28" s="8" t="s">
-        <v>357</v>
+        <v>20</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
-        <v>44411.616377314815</v>
+        <v>44409.75885416667</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>259</v>
+        <v>165</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>16</v>
@@ -3016,192 +3228,188 @@
       <c r="H29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="I29" s="2"/>
       <c r="J29" s="2" t="s">
-        <v>260</v>
+        <v>30</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>261</v>
+        <v>166</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>262</v>
+        <v>167</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>263</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
-        <v>44413.04755787037</v>
+        <v>44396.99490740741</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>111</v>
+        <v>169</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>340</v>
+        <v>171</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>16</v>
+        <v>152</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="H30" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="B31" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="N30" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="O30" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="P30" s="2" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="A31" s="3">
-        <v>44404.80846064815</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>365</v>
-      </c>
       <c r="J31" s="2" t="s">
-        <v>366</v>
+        <v>458</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>367</v>
+        <v>459</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>31</v>
+        <v>460</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N31" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>369</v>
+        <v>60</v>
+      </c>
+      <c r="N31" t="s">
+        <v>471</v>
+      </c>
+      <c r="O31" s="9" t="s">
+        <v>461</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>370</v>
+        <v>462</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
-        <v>44396.959282407406</v>
+        <v>44397.883923611109</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>37</v>
+        <v>235</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>335</v>
+        <v>236</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>16</v>
+        <v>181</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>336</v>
+        <v>18</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I32" s="2"/>
+      <c r="I32" s="2" t="s">
+        <v>237</v>
+      </c>
       <c r="J32" s="2" t="s">
-        <v>25</v>
+        <v>238</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>337</v>
+        <v>239</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>338</v>
+        <v>240</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N32" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="O32" s="5" t="s">
-        <v>146</v>
+      <c r="N32" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>242</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>339</v>
+        <v>243</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
-        <v>44410.840196759258</v>
+        <v>44411.590104166666</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>149</v>
+        <v>14</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>152</v>
+        <v>16</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>43</v>
@@ -3210,288 +3418,736 @@
         <v>29</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>358</v>
+        <v>160</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N33" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="O33" s="2" t="s">
-        <v>157</v>
+        <v>20</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O33" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
-        <v>44397.036516203705</v>
+        <v>44411.026041666664</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>190</v>
+        <v>106</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>191</v>
+        <v>15</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>192</v>
+        <v>330</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>152</v>
+        <v>42</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>193</v>
+        <v>38</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2" t="s">
-        <v>51</v>
+        <v>331</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>194</v>
+        <v>332</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>44</v>
+        <v>333</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N34" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="O34" s="2" t="s">
-        <v>196</v>
+        <v>53</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="O34" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>197</v>
+        <v>334</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
-        <v>44411.776064814818</v>
+        <v>44399.908993055556</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>264</v>
+        <v>67</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>265</v>
+        <v>68</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>266</v>
+        <v>244</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>181</v>
+        <v>48</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>267</v>
+        <v>18</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I35" s="2"/>
+      <c r="I35" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="J35" s="2" t="s">
-        <v>268</v>
+        <v>245</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>359</v>
+        <v>246</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>44</v>
+        <v>247</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="N35" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="O35" s="2" t="s">
-        <v>270</v>
+        <v>36</v>
+      </c>
+      <c r="N35" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="O35" s="5" t="s">
+        <v>142</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>271</v>
+        <v>248</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
-        <v>44405.648368055554</v>
+        <v>44409.99291666667</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>315</v>
+        <v>229</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>316</v>
+        <v>230</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>317</v>
+        <v>231</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>152</v>
+        <v>181</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>318</v>
+        <v>109</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I36" s="2" t="s">
-        <v>209</v>
-      </c>
+      <c r="I36" s="2"/>
       <c r="J36" s="2" t="s">
-        <v>319</v>
+        <v>386</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>320</v>
+        <v>387</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>321</v>
+        <v>31</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>322</v>
+        <v>232</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>323</v>
+        <v>233</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>324</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
-        <v>44396.946180555555</v>
+        <v>44397.626064814816</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>272</v>
+        <v>112</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>273</v>
+        <v>113</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>274</v>
+        <v>354</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>152</v>
+        <v>16</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="I37" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>355</v>
+      </c>
       <c r="J37" s="2" t="s">
-        <v>276</v>
+        <v>88</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>277</v>
+        <v>391</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>278</v>
+        <v>356</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N37" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="O37" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>281</v>
+        <v>26</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="O37" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="P37" s="8" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
-        <v>44411.033541666664</v>
+        <v>44411.616377314815</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>186</v>
+        <v>259</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I38" s="2"/>
+      <c r="I38" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="J38" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O38" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="3">
+        <v>44413.04755787037</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N39" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="O39" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="3">
+        <v>44404.80846064815</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="P40" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="3">
+        <v>44396.959282407406</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O41" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="3">
+        <v>44410.840196759258</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="N42" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="3">
+        <v>44397.036516203705</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N43" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="O43" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="P43" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="3">
+        <v>44411.776064814818</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="N44" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="3">
+        <v>44405.648368055554</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N45" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="3">
+        <v>44396.946180555555</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N46" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="O46" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="3">
+        <v>44411.033541666664</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="K38" s="2" t="s">
+      <c r="K47" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="L38" s="2" t="s">
+      <c r="L47" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="M38" s="2" t="s">
+      <c r="M47" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="N38" s="1" t="s">
+      <c r="N47" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O38" s="5" t="s">
+      <c r="O47" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="P38" s="2" t="s">
+      <c r="P47" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="P39" s="2"/>
-    </row>
-    <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="P40" s="2"/>
-    </row>
-    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="P41" s="2"/>
+    <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L48" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P41">
-    <sortCondition ref="C2:C41"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P47">
+    <sortCondition ref="C2:C47"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="O21" r:id="rId1" xr:uid="{9E307C65-887C-5044-8DB8-E71EB3F10045}"/>
+    <hyperlink ref="O11" r:id="rId2" xr:uid="{4A81FE9A-EBAB-0747-B2F3-61D7490B1D68}"/>
+    <hyperlink ref="O16" r:id="rId3" xr:uid="{448DA057-37C3-3B4D-9D30-C27C2FD902D3}"/>
+    <hyperlink ref="L17" r:id="rId4" xr:uid="{D8ACD1FD-B89B-654B-826E-8D368DB2BCFA}"/>
+    <hyperlink ref="O22" r:id="rId5" xr:uid="{85DCA030-31D8-4740-B777-FBA97285460E}"/>
+    <hyperlink ref="O9" r:id="rId6" xr:uid="{210441B6-FCEF-2242-865A-79AA00B99D15}"/>
+    <hyperlink ref="O27" r:id="rId7" xr:uid="{5A40EFE8-502D-2149-ACBE-311EA5579DF3}"/>
+    <hyperlink ref="O14" r:id="rId8" xr:uid="{7E0B92DD-CBCC-8F46-B940-A199BDE9BF18}"/>
+    <hyperlink ref="O25" r:id="rId9" xr:uid="{6A6E0364-629D-FF44-817A-6C9F4E3C32C0}"/>
+    <hyperlink ref="O31" r:id="rId10" xr:uid="{7DAAB33D-9347-8F48-A5B6-88CA9022F3F4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated directors and added andrew doan
</commit_message>
<xml_diff>
--- a/src/data/summer21/bios_summer21.xlsx
+++ b/src/data/summer21/bios_summer21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brennenwong/Documents/DSP Website/src/data/summer21/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Droo\DoT\dspuci-website-gatsby\src\data\summer21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C88D682-CB45-DB42-BBEC-154F3FCC27E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1FAF61-34A8-455D-A6E9-AA7C61692515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13580" yWindow="500" windowWidth="15220" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="466">
   <si>
     <t>Timestamp</t>
   </si>
@@ -367,15 +367,6 @@
     <t>https://www.linkedin.com/in/tiffany-than/</t>
   </si>
   <si>
-    <t>Cody</t>
-  </si>
-  <si>
-    <t>Enokida</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/codyenokida/</t>
-  </si>
-  <si>
     <t>Mark</t>
   </si>
   <si>
@@ -415,9 +406,6 @@
     <t>lisadeng@ucidsp.com</t>
   </si>
   <si>
-    <t>codyenokida@ucidsp.com</t>
-  </si>
-  <si>
     <t>gracehsiang@ucidsp.com</t>
   </si>
   <si>
@@ -629,15 +617,6 @@
   </si>
   <si>
     <t>Hello! My name is Brian and I initiated in the fall of my sophomore year. My favorite pastimes include playing basketball, watching movies, (attempting to become competent at) skateboarding, and spending time with friends. I also enjoy trying new foods and activities. Ask me about my interest in strategy games at recruitment!</t>
-  </si>
-  <si>
-    <t>cody_enokida</t>
-  </si>
-  <si>
-    <t>Software Engineering Intern at Beyond Limits AI</t>
-  </si>
-  <si>
-    <t>Hi there, I’m Cody Enokida and I initiated the fall quarter of my freshman year. Currently working and learning all about Web 3.0 and borderless payments; Hit me up if you’re interested about that! In my free time, I love to go outdoors, hammock, and surf.</t>
   </si>
   <si>
     <t>Darren</t>
@@ -1413,6 +1392,33 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/winnie-qi21/</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Doan</t>
+  </si>
+  <si>
+    <t>andrew_doan</t>
+  </si>
+  <si>
+    <t>Product Design/Management</t>
+  </si>
+  <si>
+    <t>Recruitment and Retention Intern at ASUCI</t>
+  </si>
+  <si>
+    <t>Product Association, ASUCI RAR</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/andrew-g-doan/</t>
+  </si>
+  <si>
+    <t>andrewdoan@ucidsp.com</t>
+  </si>
+  <si>
+    <t>Hey! My name is Andrew Doan and I initiated in Fall 2021 with the Alpha Mus. Professionally, I'm super interested in all things product. Beyond that, I love dance, art, poetry, music festivals, traveling, and good company. Looking forward to meeting you at recruitment :)</t>
   </si>
 </sst>
 </file>
@@ -1829,30 +1835,30 @@
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="5" width="21.5" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" customWidth="1"/>
+    <col min="2" max="2" width="21.36328125" customWidth="1"/>
+    <col min="3" max="5" width="21.453125" customWidth="1"/>
+    <col min="6" max="6" width="25.6328125" customWidth="1"/>
     <col min="7" max="7" width="46" customWidth="1"/>
-    <col min="8" max="8" width="40.83203125" customWidth="1"/>
-    <col min="9" max="9" width="45.5" customWidth="1"/>
-    <col min="10" max="10" width="83.33203125" customWidth="1"/>
-    <col min="11" max="11" width="96.6640625" customWidth="1"/>
-    <col min="12" max="12" width="21.5" customWidth="1"/>
-    <col min="13" max="13" width="24.1640625" customWidth="1"/>
-    <col min="14" max="14" width="36.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="23" width="21.5" customWidth="1"/>
+    <col min="8" max="8" width="40.81640625" customWidth="1"/>
+    <col min="9" max="9" width="45.453125" customWidth="1"/>
+    <col min="10" max="10" width="83.36328125" customWidth="1"/>
+    <col min="11" max="11" width="96.6328125" customWidth="1"/>
+    <col min="12" max="12" width="21.453125" customWidth="1"/>
+    <col min="13" max="13" width="24.1796875" customWidth="1"/>
+    <col min="14" max="14" width="36.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="23" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1863,7 +1869,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -1896,13 +1902,13 @@
         <v>12</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44396.977627314816</v>
       </c>
@@ -1913,7 +1919,7 @@
         <v>57</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>16</v>
@@ -1929,13 +1935,13 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>60</v>
@@ -1944,43 +1950,43 @@
         <v>61</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44404.516250000001</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>35</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>31</v>
@@ -1989,16 +1995,16 @@
         <v>104</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44409.634976851848</v>
       </c>
@@ -2009,7 +2015,7 @@
         <v>100</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -2027,13 +2033,13 @@
         <v>102</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>60</v>
@@ -2042,27 +2048,27 @@
         <v>103</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44404.857893518521</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>17</v>
@@ -2075,28 +2081,28 @@
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44397.64371527778</v>
       </c>
@@ -2107,7 +2113,7 @@
         <v>63</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>48</v>
@@ -2126,10 +2132,10 @@
         <v>51</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>65</v>
@@ -2138,13 +2144,13 @@
         <v>66</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44416.612488425926</v>
       </c>
@@ -2155,7 +2161,7 @@
         <v>96</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>42</v>
@@ -2171,10 +2177,10 @@
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>31</v>
@@ -2186,33 +2192,33 @@
         <v>98</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44404.653217592589</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>50</v>
@@ -2222,84 +2228,84 @@
         <v>51</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>65</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44397.382604166669</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>115</v>
+        <v>457</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>116</v>
+        <v>458</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>203</v>
+        <v>459</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>42</v>
+        <v>388</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>23</v>
+        <v>389</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>64</v>
+        <v>356</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>51</v>
+        <v>460</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>204</v>
+        <v>461</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>31</v>
+        <v>462</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>131</v>
+        <v>20</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>464</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>43</v>
@@ -2314,92 +2320,92 @@
         <v>102</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>53</v>
       </c>
       <c r="N10" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>44396.99622685185</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>44397.802523148152</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>17</v>
@@ -2412,10 +2418,10 @@
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>31</v>
@@ -2424,39 +2430,39 @@
         <v>89</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>31</v>
@@ -2468,16 +2474,16 @@
         <v>20</v>
       </c>
       <c r="N13" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44404.873078703706</v>
       </c>
@@ -2488,7 +2494,7 @@
         <v>81</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>42</v>
@@ -2504,13 +2510,13 @@
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>39</v>
@@ -2519,68 +2525,68 @@
         <v>82</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="P14" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="13" x14ac:dyDescent="0.15">
-      <c r="B15" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>395</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>65</v>
       </c>
       <c r="N15" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>44396.943645833337</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>42</v>
@@ -2599,7 +2605,7 @@
         <v>25</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="L16" s="9" t="s">
         <v>74</v>
@@ -2611,13 +2617,13 @@
         <v>75</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="P16" s="6" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>44042.649953703702</v>
       </c>
@@ -2628,7 +2634,7 @@
         <v>47</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>48</v>
@@ -2647,7 +2653,7 @@
         <v>51</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>52</v>
@@ -2659,27 +2665,27 @@
         <v>54</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>44398.992349537039</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>43</v>
@@ -2691,31 +2697,31 @@
         <v>35</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>44398.099432870367</v>
       </c>
@@ -2726,7 +2732,7 @@
         <v>87</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>42</v>
@@ -2738,17 +2744,17 @@
         <v>38</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>89</v>
@@ -2757,36 +2763,36 @@
         <v>90</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>392</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>399</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>31</v>
@@ -2798,60 +2804,60 @@
         <v>53</v>
       </c>
       <c r="N20" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>53</v>
       </c>
       <c r="N21" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>44404.807638888888</v>
       </c>
@@ -2862,7 +2868,7 @@
         <v>92</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>16</v>
@@ -2883,10 +2889,10 @@
         <v>30</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>65</v>
@@ -2895,24 +2901,24 @@
         <v>94</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>44046.843055555553</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>48</v>
@@ -2921,81 +2927,81 @@
         <v>43</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>53</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>35</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>89</v>
       </c>
       <c r="N24" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="O24" s="9" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>44410.679201388892</v>
       </c>
@@ -3006,7 +3012,7 @@
         <v>77</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>42</v>
@@ -3015,20 +3021,20 @@
         <v>23</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>78</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>53</v>
@@ -3037,77 +3043,77 @@
         <v>79</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N26" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>44410.762546296297</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>35</v>
@@ -3117,7 +3123,7 @@
         <v>30</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>31</v>
@@ -3126,16 +3132,16 @@
         <v>20</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>44409.75885416667</v>
       </c>
@@ -3146,7 +3152,7 @@
         <v>28</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>16</v>
@@ -3165,10 +3171,10 @@
         <v>30</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>32</v>
@@ -3177,27 +3183,27 @@
         <v>33</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>44396.99490740741</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>17</v>
@@ -3209,75 +3215,75 @@
         <v>78</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>70</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>60</v>
       </c>
       <c r="N30" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="O30" s="9" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>44397.883923611109</v>
       </c>
@@ -3285,13 +3291,13 @@
         <v>67</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>23</v>
@@ -3303,31 +3309,31 @@
         <v>35</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>44411.590104166666</v>
       </c>
@@ -3338,7 +3344,7 @@
         <v>15</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>16</v>
@@ -3353,16 +3359,16 @@
         <v>19</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>20</v>
@@ -3371,13 +3377,13 @@
         <v>21</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>44411.026041666664</v>
       </c>
@@ -3388,7 +3394,7 @@
         <v>15</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>42</v>
@@ -3404,13 +3410,13 @@
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>53</v>
@@ -3419,13 +3425,13 @@
         <v>107</v>
       </c>
       <c r="O33" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>44399.908993055556</v>
       </c>
@@ -3436,7 +3442,7 @@
         <v>68</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>48</v>
@@ -3454,13 +3460,13 @@
         <v>69</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>36</v>
@@ -3469,27 +3475,27 @@
         <v>71</v>
       </c>
       <c r="O34" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>44409.99291666667</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>17</v>
@@ -3502,10 +3508,10 @@
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>31</v>
@@ -3514,16 +3520,16 @@
         <v>104</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>44397.626064814816</v>
       </c>
@@ -3534,7 +3540,7 @@
         <v>113</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>16</v>
@@ -3549,16 +3555,16 @@
         <v>24</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>26</v>
@@ -3567,13 +3573,13 @@
         <v>114</v>
       </c>
       <c r="O36" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="P36" s="8" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>44411.616377314815</v>
       </c>
@@ -3584,7 +3590,7 @@
         <v>83</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>16</v>
@@ -3602,13 +3608,13 @@
         <v>84</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="M37" s="2" t="s">
         <v>53</v>
@@ -3617,13 +3623,13 @@
         <v>85</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>44413.04755787037</v>
       </c>
@@ -3631,10 +3637,10 @@
         <v>111</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>16</v>
@@ -3650,60 +3656,60 @@
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>89</v>
       </c>
       <c r="N38" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="O38" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>44404.80846064815</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="L39" s="2" t="s">
         <v>31</v>
@@ -3712,16 +3718,16 @@
         <v>36</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>44396.959282407406</v>
       </c>
@@ -3732,7 +3738,7 @@
         <v>37</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>16</v>
@@ -3741,7 +3747,7 @@
         <v>43</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>35</v>
@@ -3751,10 +3757,10 @@
         <v>25</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>26</v>
@@ -3763,27 +3769,27 @@
         <v>110</v>
       </c>
       <c r="O40" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>44410.840196759258</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>43</v>
@@ -3795,51 +3801,51 @@
         <v>24</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>104</v>
       </c>
       <c r="N41" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>44397.036516203705</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>50</v>
@@ -3849,7 +3855,7 @@
         <v>51</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="L42" s="2" t="s">
         <v>44</v>
@@ -3858,128 +3864,128 @@
         <v>26</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>44411.776064814818</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>44</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="N43" s="4" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>44405.648368055554</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>35</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="M44" s="2" t="s">
         <v>53</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44396.946180555555</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>43</v>
@@ -3988,32 +3994,32 @@
         <v>38</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="M45" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N45" s="4" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>44411.033541666664</v>
       </c>
@@ -4024,7 +4030,7 @@
         <v>41</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>42</v>
@@ -4040,28 +4046,28 @@
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="N46" s="1" t="s">
         <v>45</v>
       </c>
       <c r="O46" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L47" s="2"/>
     </row>
   </sheetData>
@@ -4078,6 +4084,8 @@
     <hyperlink ref="O13" r:id="rId7" xr:uid="{7E0B92DD-CBCC-8F46-B940-A199BDE9BF18}"/>
     <hyperlink ref="O24" r:id="rId8" xr:uid="{6A6E0364-629D-FF44-817A-6C9F4E3C32C0}"/>
     <hyperlink ref="O30" r:id="rId9" xr:uid="{7DAAB33D-9347-8F48-A5B6-88CA9022F3F4}"/>
+    <hyperlink ref="N9" r:id="rId10" xr:uid="{3FEE33F3-63FD-49C4-92AB-1042A2591AA6}"/>
+    <hyperlink ref="O9" r:id="rId11" xr:uid="{7CBE67B6-B9B5-45EE-9470-F4AA5E5FF358}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
took out recruitment page, added proweek page, updated proweek page, updated sample case study, added alphamu pics + retakes
</commit_message>
<xml_diff>
--- a/src/data/summer21/bios_summer21.xlsx
+++ b/src/data/summer21/bios_summer21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Droo\DoT\dspuci-website-gatsby\src\data\summer21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1FAF61-34A8-455D-A6E9-AA7C61692515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30333050-0AD3-43F6-A0FC-A8103542DB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1409,16 +1409,16 @@
     <t>Recruitment and Retention Intern at ASUCI</t>
   </si>
   <si>
-    <t>Product Association, ASUCI RAR</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/andrew-g-doan/</t>
   </si>
   <si>
     <t>andrewdoan@ucidsp.com</t>
   </si>
   <si>
-    <t>Hey! My name is Andrew Doan and I initiated in Fall 2021 with the Alpha Mus. Professionally, I'm super interested in all things product. Beyond that, I love dance, art, poetry, music festivals, traveling, and good company. Looking forward to meeting you at recruitment :)</t>
+    <t>Product Association, ASUCI</t>
+  </si>
+  <si>
+    <t>Hello, my name is Andrew Doan and I initiated in Fall 2021 with the Alpha Mus! Professionally, I'm super interested in all things product. Beyond that, I love dance, art, poetry, music festivals, traveling, and good company. Looking forward to meeting you at recruitment :)</t>
   </si>
 </sst>
 </file>
@@ -1835,7 +1835,7 @@
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
@@ -2279,16 +2279,16 @@
         <v>461</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N9" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="O9" s="9" t="s">
         <v>463</v>
-      </c>
-      <c r="O9" s="9" t="s">
-        <v>464</v>
       </c>
       <c r="P9" s="2" t="s">
         <v>465</v>

</xml_diff>

<commit_message>
fixed pictures + presidents letter
</commit_message>
<xml_diff>
--- a/src/data/summer21/bios_summer21.xlsx
+++ b/src/data/summer21/bios_summer21.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Droo\DoT\dspuci-website-gatsby\src\data\summer21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30333050-0AD3-43F6-A0FC-A8103542DB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357753A9-AD76-484D-8324-1758ECB1A814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1418,7 +1418,7 @@
     <t>Product Association, ASUCI</t>
   </si>
   <si>
-    <t>Hello, my name is Andrew Doan and I initiated in Fall 2021 with the Alpha Mus! Professionally, I'm super interested in all things product. Beyond that, I love dance, art, poetry, music festivals, traveling, and good company. Looking forward to meeting you at recruitment :)</t>
+    <t>Hello!! My name is Andrew Doan and I initiated in Fall 2021 with the Alpha Mus! Professionally, I'm super interested in all things product. Beyond that, I love dance, art, poetry, music festivals, traveling, and good company. Looking forward to meeting you at recruitment :)</t>
   </si>
 </sst>
 </file>
@@ -1835,7 +1835,7 @@
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="P9" sqref="P9"/>

</xml_diff>

<commit_message>
updated bios, vppe pic
</commit_message>
<xml_diff>
--- a/src/data/summer21/bios_summer21.xlsx
+++ b/src/data/summer21/bios_summer21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Droo\DoT\dspuci-website-gatsby\src\data\summer21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7710B21-A575-4307-8279-595DD1CD60ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20DDCF9-C151-4FA3-AEC7-7E4B34227F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="418">
   <si>
     <t>Timestamp</t>
   </si>
@@ -196,9 +196,6 @@
     <t>Informatics</t>
   </si>
   <si>
-    <t>Product Management</t>
-  </si>
-  <si>
     <t>Jeon</t>
   </si>
   <si>
@@ -601,9 +598,6 @@
     <t>dylantanzil@ucidsp.com</t>
   </si>
   <si>
-    <t>Hi! My name is Dylan, and I initiated in the spring quarter of my first year. In my free time, I enjoy playing basketball, skiing, snowboarding, and going on cool adventures. I am currently learning how to electric skateboard, and I have surprisingly not fallen down yet! Feel free to ask me about cars, options trading, food cuisines, and anything that excites you. I am looking forward to meeting you!</t>
-  </si>
-  <si>
     <t>Ros</t>
   </si>
   <si>
@@ -662,12 +656,6 @@
   </si>
   <si>
     <t>Investment Banking Summer Analyst at Deutsche Bank</t>
-  </si>
-  <si>
-    <t>MUSA Vice President of Finance, ASUCI Financial Wellness Commission, MAISS</t>
-  </si>
-  <si>
-    <t>My name is Grace and I initiated fall my freshman year with the Alpha Iotas! I'm extremely stoked to meet all of you and ask me about my favorite books, work life balance, night life in NY, independent travel, and fashion! Reach out with any questions, would love to chat :)</t>
   </si>
   <si>
     <t>Jenny</t>
@@ -1004,15 +992,6 @@
     <t>Investment Analyst Intern at Interlink Global Investments</t>
   </si>
   <si>
-    <t>Consulting, Sales, Marketing</t>
-  </si>
-  <si>
-    <t>Sales Partner at UpMerch</t>
-  </si>
-  <si>
-    <t>Hi, I'm Grace and I initiated in fall quarter of my 1st year with the Alpha Eta class. When I have free time, I'm usually trying new recipes, finding new music on Soundcloud, or adventuring in search of new food/coffee/views. A fun fact about me is that my a capella group in high school sang the National Anthem at a Warriors game. Ask me about my puppy or the places I've traveled to at recruitment!</t>
-  </si>
-  <si>
     <t>Social Media Intern at J.ING</t>
   </si>
   <si>
@@ -1269,13 +1248,40 @@
   </si>
   <si>
     <t>MUSA, Product Association, Previous: AMP Mentee</t>
+  </si>
+  <si>
+    <t>Product Management, VC</t>
+  </si>
+  <si>
+    <t>President @ MUSA, MAISS, ASUCI Financial Wellness Commission</t>
+  </si>
+  <si>
+    <t>My name is Grace and I initiated fall my freshman year with the Alpha Iotas! I'm extremely stoked to meet all of you :) Ask me about my favorite books, work life balance, rollerskating, night life in NY, travel, makeup and fashion! Reach out with any questions, would love to chat!</t>
+  </si>
+  <si>
+    <t>Venture Capital and Business Analytic Extern at HP Tech Ventures</t>
+  </si>
+  <si>
+    <t>Real Estate Association, Sigma Chi, RUF</t>
+  </si>
+  <si>
+    <t>UBA, SGSM</t>
+  </si>
+  <si>
+    <t>Hi!! I'm Grace and I initiated in fall quarter of 2018 with the Alpha Eta class. When I have free time, I'm usually trying new recipes, finding new music on Soundcloud, or adventuring in search of new food/coffee/views. A fun fact about me is that my a capella group in high school sang the National Anthem at a Warriors game. Ask me about my puppy or the places I've traveled to at recruitment :")</t>
+  </si>
+  <si>
+    <t>Hi! My name is Dylan, and I initiated in the spring quarter of my first year. In my free time, I enjoy playing volleyball, basketball, and Valorant. Feel free to ask me about cars, options trading, and random stuff. Looking forward to seeing you :)</t>
+  </si>
+  <si>
+    <t>Intern at Linda S. Congleton &amp; Associates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1328,6 +1334,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1350,7 +1362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1359,11 +1371,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1685,10 +1700,10 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22:XFD22"/>
+      <selection pane="bottomRight" activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1719,7 +1734,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -1752,7 +1767,7 @@
         <v>12</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>13</v>
@@ -1769,7 +1784,7 @@
         <v>49</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>16</v>
@@ -1785,13 +1800,13 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>52</v>
@@ -1800,10 +1815,10 @@
         <v>53</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -1811,47 +1826,47 @@
         <v>44404.516250000001</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>35</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N3" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -1859,13 +1874,13 @@
         <v>44409.634976851848</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -1874,34 +1889,34 @@
         <v>41</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>52</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -1909,16 +1924,16 @@
         <v>44404.857893518521</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>17</v>
@@ -1931,25 +1946,25 @@
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -1957,22 +1972,22 @@
         <v>44404.653217592589</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>45</v>
@@ -1982,22 +1997,22 @@
         <v>46</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>55</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -2005,94 +2020,94 @@
         <v>44397.382604166669</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>57</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N7" s="9" t="s">
-        <v>407</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>408</v>
+      <c r="N7" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>401</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>35</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N8" t="s">
-        <v>398</v>
-      </c>
-      <c r="O8" s="10" t="s">
-        <v>348</v>
+        <v>391</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>341</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -2100,49 +2115,49 @@
         <v>44396.99622685185</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I9" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N9" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="O9" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="P9" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -2150,16 +2165,16 @@
         <v>44397.802523148152</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>17</v>
@@ -2172,51 +2187,51 @@
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>31</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>31</v>
@@ -2228,13 +2243,13 @@
         <v>20</v>
       </c>
       <c r="N11" t="s">
-        <v>397</v>
-      </c>
-      <c r="O11" s="9" t="s">
-        <v>377</v>
+        <v>390</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>370</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -2242,13 +2257,13 @@
         <v>44404.873078703706</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>40</v>
@@ -2264,69 +2279,69 @@
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>329</v>
+        <v>415</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>55</v>
       </c>
       <c r="N13" t="s">
-        <v>396</v>
-      </c>
-      <c r="O13" s="9" t="s">
-        <v>355</v>
+        <v>389</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>348</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -2334,13 +2349,13 @@
         <v>44396.943645833337</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>40</v>
@@ -2349,7 +2364,7 @@
         <v>23</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>24</v>
@@ -2359,22 +2374,22 @@
         <v>25</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>61</v>
+        <v>203</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P14" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -2382,49 +2397,49 @@
         <v>44398.992349537039</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>35</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K15" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -2432,13 +2447,13 @@
         <v>44398.099432870367</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>40</v>
@@ -2450,120 +2465,123 @@
         <v>38</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="M16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K16" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="M16" s="2" t="s">
+      <c r="N16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="N16" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="O16" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>31</v>
+      <c r="K17" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>413</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N17" t="s">
-        <v>394</v>
-      </c>
-      <c r="O17" s="9" t="s">
-        <v>341</v>
+        <v>387</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>334</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N18" t="s">
-        <v>395</v>
-      </c>
-      <c r="O18" s="9" t="s">
-        <v>363</v>
+        <v>388</v>
+      </c>
+      <c r="O18" s="8" t="s">
+        <v>356</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -2571,13 +2589,13 @@
         <v>44404.807638888888</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>16</v>
@@ -2586,34 +2604,34 @@
         <v>41</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>55</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -2621,13 +2639,13 @@
         <v>44046.843055555553</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>43</v>
@@ -2636,122 +2654,122 @@
         <v>41</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N20" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="P20" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="O20" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>35</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N21" t="s">
-        <v>399</v>
-      </c>
-      <c r="O21" s="9" t="s">
-        <v>385</v>
+        <v>392</v>
+      </c>
+      <c r="O21" s="8" t="s">
+        <v>378</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N22" t="s">
-        <v>400</v>
-      </c>
-      <c r="O22" s="9" t="s">
-        <v>370</v>
+        <v>393</v>
+      </c>
+      <c r="O22" s="8" t="s">
+        <v>363</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2759,22 +2777,22 @@
         <v>44410.762546296297</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>150</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>35</v>
@@ -2784,7 +2802,7 @@
         <v>30</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>31</v>
@@ -2793,13 +2811,13 @@
         <v>20</v>
       </c>
       <c r="N23" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="O23" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="O23" s="2" t="s">
+      <c r="P23" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -2813,7 +2831,7 @@
         <v>28</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>16</v>
@@ -2832,10 +2850,10 @@
         <v>30</v>
       </c>
       <c r="K24" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="L24" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>32</v>
@@ -2844,10 +2862,10 @@
         <v>33</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -2855,16 +2873,16 @@
         <v>44396.99490740741</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="E25" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>17</v>
@@ -2873,75 +2891,75 @@
         <v>54</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I25" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="L25" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N25" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="O25" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="O25" s="2" t="s">
+      <c r="P25" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>52</v>
       </c>
       <c r="N26" t="s">
-        <v>401</v>
-      </c>
-      <c r="O26" s="9" t="s">
-        <v>392</v>
+        <v>394</v>
+      </c>
+      <c r="O26" s="8" t="s">
+        <v>385</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -2952,13 +2970,13 @@
         <v>56</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>23</v>
@@ -2970,28 +2988,28 @@
         <v>35</v>
       </c>
       <c r="I27" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K27" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="L27" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>199</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N27" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="P27" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="O27" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -3005,7 +3023,7 @@
         <v>15</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>16</v>
@@ -3020,16 +3038,16 @@
         <v>19</v>
       </c>
       <c r="I28" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="K28" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="L28" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>20</v>
@@ -3038,10 +3056,10 @@
         <v>21</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
@@ -3049,13 +3067,13 @@
         <v>44411.026041666664</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>40</v>
@@ -3071,25 +3089,25 @@
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3097,47 +3115,47 @@
         <v>44409.99291666667</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="E30" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>35</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2" t="s">
-        <v>327</v>
+        <v>310</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>328</v>
+        <v>417</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>31</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N30" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="O30" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="O30" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="P30" s="2" t="s">
-        <v>193</v>
+        <v>416</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3145,13 +3163,13 @@
         <v>44397.626064814816</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="D31" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>16</v>
@@ -3166,28 +3184,28 @@
         <v>24</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="P31" s="8" t="s">
-        <v>305</v>
+        <v>113</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3195,13 +3213,13 @@
         <v>44411.616377314815</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>16</v>
@@ -3216,28 +3234,28 @@
         <v>24</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>214</v>
+        <v>410</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>215</v>
+        <v>411</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3245,13 +3263,13 @@
         <v>44413.04755787037</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>16</v>
@@ -3260,32 +3278,32 @@
         <v>41</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O33" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3293,49 +3311,49 @@
         <v>44404.80846064815</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G34" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="K34" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>315</v>
-      </c>
       <c r="L34" s="2" t="s">
-        <v>31</v>
+        <v>414</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>36</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3343,13 +3361,13 @@
         <v>44396.959282407406</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>16</v>
@@ -3358,7 +3376,7 @@
         <v>41</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>35</v>
@@ -3368,22 +3386,22 @@
         <v>25</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O35" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3391,16 +3409,16 @@
         <v>44410.840196759258</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>41</v>
@@ -3412,28 +3430,28 @@
         <v>24</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="J36" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="K36" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K36" s="2" t="s">
+      <c r="L36" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="L36" s="2" t="s">
+      <c r="M36" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="N36" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="M36" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="N36" s="4" t="s">
+      <c r="O36" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="O36" s="2" t="s">
+      <c r="P36" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="P36" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3441,22 +3459,22 @@
         <v>44397.036516203705</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="E37" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>45</v>
@@ -3466,7 +3484,7 @@
         <v>46</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>42</v>
@@ -3475,13 +3493,13 @@
         <v>26</v>
       </c>
       <c r="N37" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="O37" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="O37" s="2" t="s">
+      <c r="P37" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3489,47 +3507,47 @@
         <v>44411.776064814818</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>42</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3537,49 +3555,49 @@
         <v>44405.648368055554</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>35</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3587,16 +3605,16 @@
         <v>44396.946180555555</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>41</v>
@@ -3605,29 +3623,29 @@
         <v>38</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3651,5 +3669,6 @@
     <hyperlink ref="O7" r:id="rId11" xr:uid="{7CBE67B6-B9B5-45EE-9470-F4AA5E5FF358}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "fixed mark bio"
This reverts commit f50ec70f536195cf816222a2a61113d4b431c418.
</commit_message>
<xml_diff>
--- a/src/data/summer21/bios_summer21.xlsx
+++ b/src/data/summer21/bios_summer21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Droo\DoT\dspuci-website-gatsby\src\data\summer21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDDA74A-DCB6-4793-BA81-D37EA7EF47E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D6E8D3-0CB1-489C-87FB-7F5A50ECB960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1703,10 +1703,10 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="Q5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2656,7 +2656,7 @@
         <v>43</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
alphabetized all brothers + vppe tba
</commit_message>
<xml_diff>
--- a/src/data/summer21/bios_summer21.xlsx
+++ b/src/data/summer21/bios_summer21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorin\dspuci-website-gatsby\src\data\summer21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810DDFD0-2E45-45E1-A2F1-65F33B1A4A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8D8B85-3103-40AC-AD49-A1A6042DB0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1735,10 +1735,10 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1857,355 +1857,351 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>44409.634976851848</v>
-      </c>
       <c r="B3" s="2" t="s">
-        <v>63</v>
+        <v>383</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>64</v>
+        <v>384</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>213</v>
+        <v>385</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>16</v>
+        <v>359</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>65</v>
+        <v>396</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>66</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>214</v>
+        <v>386</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>215</v>
+        <v>387</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>216</v>
+        <v>388</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>86</v>
+        <v>68</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>390</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>217</v>
+        <v>391</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>44404.857893518521</v>
+        <v>44409.634976851848</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>192</v>
+        <v>63</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>193</v>
+        <v>64</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="J4" s="2" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>197</v>
+        <v>216</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>199</v>
+        <v>48</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>200</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>44404.653217592589</v>
+        <v>44404.857893518521</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>228</v>
+        <v>192</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>229</v>
+        <v>193</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>230</v>
+        <v>194</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>231</v>
+        <v>34</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>45</v>
+        <v>195</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>232</v>
+        <v>196</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>233</v>
+        <v>197</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>234</v>
+        <v>198</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>235</v>
+        <v>199</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>236</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>44397.382604166669</v>
-      </c>
       <c r="B6" s="2" t="s">
-        <v>329</v>
+        <v>356</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>330</v>
+        <v>357</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>331</v>
+        <v>358</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>265</v>
+        <v>359</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>246</v>
+        <v>18</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>51</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>352</v>
+        <v>364</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>334</v>
+        <v>365</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>332</v>
+        <v>362</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>333</v>
+        <v>363</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>353</v>
+        <v>366</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>271</v>
+        <v>413</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>272</v>
+        <v>357</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>273</v>
+        <v>414</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>265</v>
+        <v>359</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>65</v>
+        <v>415</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N7" t="s">
-        <v>325</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>44396.99622685185</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="J8" s="2" t="s">
-        <v>139</v>
+        <v>378</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>140</v>
+        <v>31</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>143</v>
+        <v>379</v>
+      </c>
+      <c r="M8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>381</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>144</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>44397.802523148152</v>
+        <v>44404.653217592589</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>254</v>
+        <v>228</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>229</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>47</v>
+        <v>231</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>256</v>
+        <v>45</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>41</v>
+        <v>233</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>257</v>
+        <v>234</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>351</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>44397.382604166669</v>
+      </c>
       <c r="B10" s="2" t="s">
-        <v>301</v>
+        <v>329</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>302</v>
+        <v>330</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>303</v>
+        <v>331</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>265</v>
@@ -2214,374 +2210,373 @@
         <v>17</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>304</v>
+        <v>246</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>24</v>
+        <v>51</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>348</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>305</v>
+        <v>352</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>31</v>
+        <v>355</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>31</v>
+        <v>334</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N10" t="s">
-        <v>324</v>
+      <c r="N10" s="7" t="s">
+        <v>332</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>306</v>
+        <v>333</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>307</v>
+        <v>353</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>279</v>
+        <v>404</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>280</v>
+        <v>405</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>265</v>
+        <v>406</v>
+      </c>
+      <c r="E11" t="s">
+        <v>359</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>282</v>
+        <v>407</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>283</v>
+        <v>408</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>291</v>
+        <v>409</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N11" t="s">
-        <v>323</v>
+        <v>26</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>410</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>284</v>
+        <v>411</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>285</v>
+        <v>412</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>44398.992349537039</v>
-      </c>
       <c r="B12" s="2" t="s">
-        <v>183</v>
+        <v>271</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>184</v>
+        <v>272</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>185</v>
+        <v>273</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>124</v>
+        <v>265</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>35</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>186</v>
+        <v>66</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>30</v>
+        <v>274</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>187</v>
+        <v>275</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>188</v>
+        <v>276</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>190</v>
+        <v>46</v>
+      </c>
+      <c r="N12" t="s">
+        <v>325</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>277</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>191</v>
+        <v>278</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>44396.99622685185</v>
+      </c>
       <c r="B13" s="2" t="s">
-        <v>262</v>
+        <v>135</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>263</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>264</v>
+        <v>136</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>265</v>
+        <v>99</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>266</v>
+        <v>137</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>267</v>
+        <v>24</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>66</v>
+        <v>138</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>343</v>
-      </c>
-      <c r="L13" s="10" t="s">
-        <v>344</v>
+        <v>139</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N13" t="s">
-        <v>321</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>270</v>
+        <v>26</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>269</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>44397.802523148152</v>
+      </c>
       <c r="B14" s="2" t="s">
-        <v>286</v>
+        <v>254</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>287</v>
+        <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>288</v>
+        <v>255</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>265</v>
+        <v>99</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>289</v>
+        <v>47</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>336</v>
-      </c>
+      <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>290</v>
+        <v>256</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>337</v>
+        <v>260</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>338</v>
+        <v>41</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N14" t="s">
-        <v>322</v>
-      </c>
-      <c r="O14" s="7" t="s">
-        <v>292</v>
+        <v>58</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>258</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>293</v>
+        <v>351</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>44404.807638888888</v>
-      </c>
       <c r="B15" s="2" t="s">
-        <v>59</v>
+        <v>301</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>60</v>
+        <v>302</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>179</v>
+        <v>303</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>16</v>
+        <v>265</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>61</v>
+        <v>304</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="J15" s="2" t="s">
-        <v>30</v>
+        <v>305</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>180</v>
+        <v>31</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>181</v>
+        <v>31</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O15" s="5" t="s">
-        <v>87</v>
+        <v>20</v>
+      </c>
+      <c r="N15" t="s">
+        <v>324</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>306</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>182</v>
+        <v>307</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>44046.843055555553</v>
-      </c>
       <c r="B16" s="2" t="s">
-        <v>77</v>
+        <v>279</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>78</v>
+        <v>280</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>201</v>
+        <v>281</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>42</v>
+        <v>265</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>79</v>
+        <v>282</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>202</v>
-      </c>
       <c r="J16" s="2" t="s">
-        <v>25</v>
+        <v>283</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>259</v>
+        <v>31</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>80</v>
+        <v>291</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="O16" s="5" t="s">
-        <v>88</v>
+        <v>50</v>
+      </c>
+      <c r="N16" t="s">
+        <v>323</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>284</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>82</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>44398.992349537039</v>
+      </c>
       <c r="B17" s="2" t="s">
-        <v>308</v>
+        <v>183</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>309</v>
+        <v>184</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>310</v>
+        <v>185</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>265</v>
+        <v>124</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>311</v>
+        <v>69</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="I17" s="2" t="s">
+        <v>186</v>
+      </c>
       <c r="J17" s="2" t="s">
-        <v>149</v>
+        <v>30</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>349</v>
+        <v>187</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>350</v>
+        <v>188</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N17" t="s">
-        <v>326</v>
-      </c>
-      <c r="O17" s="7" t="s">
-        <v>313</v>
+        <v>126</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>312</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>294</v>
+        <v>262</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>295</v>
+        <v>263</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>296</v>
+        <v>264</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>265</v>
@@ -2590,149 +2585,151 @@
         <v>17</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>125</v>
+        <v>266</v>
       </c>
       <c r="H18" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="L18" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N18" t="s">
+        <v>321</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="E19" t="s">
+        <v>359</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N18" t="s">
-        <v>327</v>
-      </c>
-      <c r="O18" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>44409.75885416667</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="I20" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N20" t="s">
+        <v>322</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>44404.807638888888</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O19" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>44396.99490740741</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="G21" s="2" t="s">
-        <v>317</v>
+        <v>61</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>24</v>
@@ -2741,187 +2738,177 @@
         <v>66</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>318</v>
+        <v>180</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>339</v>
+        <v>181</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="N21" t="s">
-        <v>328</v>
-      </c>
-      <c r="O21" s="7" t="s">
-        <v>319</v>
+        <v>50</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>320</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>44411.590104166666</v>
+        <v>44046.843055555553</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>106</v>
+        <v>201</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>107</v>
+        <v>202</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>108</v>
+        <v>25</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>109</v>
+        <v>259</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>21</v>
+        <v>46</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>44409.99291666667</v>
-      </c>
       <c r="B23" s="2" t="s">
-        <v>153</v>
+        <v>308</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>154</v>
+        <v>309</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>155</v>
+        <v>310</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>124</v>
+        <v>265</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>71</v>
+        <v>311</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I23" s="2"/>
       <c r="J23" s="2" t="s">
-        <v>249</v>
+        <v>149</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>31</v>
+        <v>350</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="N23" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
+      </c>
+      <c r="N23" t="s">
+        <v>326</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>313</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>346</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>44397.626064814816</v>
-      </c>
       <c r="B24" s="2" t="s">
-        <v>74</v>
+        <v>294</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>75</v>
+        <v>295</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>237</v>
+        <v>296</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>16</v>
+        <v>265</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>43</v>
+        <v>125</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="J24" s="2" t="s">
-        <v>57</v>
+        <v>297</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>261</v>
+        <v>31</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>239</v>
+        <v>298</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="O24" s="5" t="s">
-        <v>91</v>
+        <v>32</v>
+      </c>
+      <c r="N24" t="s">
+        <v>327</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>299</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>240</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>44411.616377314815</v>
+        <v>44409.75885416667</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>16</v>
@@ -2935,141 +2922,138 @@
       <c r="H25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="I25" s="2"/>
       <c r="J25" s="2" t="s">
-        <v>159</v>
+        <v>30</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>160</v>
+        <v>113</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>341</v>
+        <v>114</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>342</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>44413.04755787037</v>
+        <v>44396.99490740741</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>223</v>
+        <v>118</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N26" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="O26" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>44404.80846064815</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>247</v>
-      </c>
       <c r="I27" s="2" t="s">
-        <v>248</v>
+        <v>66</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>249</v>
+        <v>100</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>250</v>
+        <v>318</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N27" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="O27" s="2" t="s">
-        <v>252</v>
+        <v>48</v>
+      </c>
+      <c r="N27" t="s">
+        <v>328</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>319</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>253</v>
+        <v>320</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>44396.959282407406</v>
+        <v>44411.590104166666</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>218</v>
+        <v>106</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>16</v>
@@ -3078,287 +3062,291 @@
         <v>23</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>219</v>
+        <v>29</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I28" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="J28" s="2" t="s">
-        <v>25</v>
+        <v>108</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>220</v>
+        <v>109</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>221</v>
+        <v>110</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>222</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>44410.840196759258</v>
+        <v>44409.99291666667</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>96</v>
+        <v>153</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>98</v>
+        <v>155</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>241</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="I29" s="2"/>
       <c r="J29" s="2" t="s">
-        <v>100</v>
+        <v>249</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>101</v>
+        <v>347</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>102</v>
+        <v>31</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>68</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>103</v>
+        <v>156</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>104</v>
+        <v>157</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>105</v>
+        <v>346</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>44397.036516203705</v>
+        <v>44397.626064814816</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>127</v>
+        <v>74</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>128</v>
+        <v>75</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>129</v>
+        <v>237</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>130</v>
+        <v>43</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I30" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>238</v>
+      </c>
       <c r="J30" s="2" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>131</v>
+        <v>261</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>41</v>
+        <v>239</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N30" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="O30" s="2" t="s">
-        <v>133</v>
+      <c r="N30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="O30" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>134</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>44411.776064814818</v>
+        <v>44411.616377314815</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>161</v>
+        <v>53</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>162</v>
+        <v>54</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>124</v>
+        <v>16</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I31" s="2"/>
+      <c r="I31" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="J31" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>242</v>
+        <v>160</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>41</v>
+        <v>341</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="N31" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>167</v>
+        <v>46</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O31" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>168</v>
+        <v>342</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>44405.648368055554</v>
+        <v>44413.04755787037</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>203</v>
+        <v>73</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>204</v>
+        <v>83</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>205</v>
+        <v>223</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>206</v>
+        <v>61</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>138</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="I32" s="2"/>
       <c r="J32" s="2" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N32" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="O32" s="2" t="s">
-        <v>211</v>
+        <v>58</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="O32" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>44396.946180555555</v>
+        <v>44404.80846064815</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>169</v>
+        <v>243</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>170</v>
+        <v>244</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>171</v>
+        <v>245</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>38</v>
+        <v>246</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="I33" s="2"/>
+        <v>247</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>248</v>
+      </c>
       <c r="J33" s="2" t="s">
-        <v>173</v>
+        <v>249</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>174</v>
+        <v>250</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>175</v>
+        <v>345</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>176</v>
+        <v>251</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>177</v>
+        <v>252</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>178</v>
+        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>357</v>
+        <v>244</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>359</v>
@@ -3367,394 +3355,406 @@
         <v>40</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>365</v>
+        <v>31</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>362</v>
+        <v>373</v>
       </c>
       <c r="O34" s="7" t="s">
-        <v>363</v>
+        <v>374</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>44396.959282407406</v>
+      </c>
       <c r="B35" s="2" t="s">
-        <v>367</v>
+        <v>70</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>244</v>
+        <v>37</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>368</v>
+        <v>218</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>359</v>
+        <v>16</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>49</v>
+        <v>219</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>369</v>
-      </c>
+      <c r="I35" s="2"/>
       <c r="J35" s="2" t="s">
-        <v>370</v>
+        <v>25</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>371</v>
+        <v>220</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>31</v>
+        <v>221</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="N35" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="O35" s="7" t="s">
-        <v>374</v>
+        <v>26</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O35" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>372</v>
+        <v>222</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>44410.840196759258</v>
+      </c>
       <c r="B36" s="2" t="s">
-        <v>375</v>
+        <v>96</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>376</v>
+        <v>97</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>377</v>
+        <v>98</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>359</v>
+        <v>99</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>66</v>
+        <v>241</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>378</v>
+        <v>100</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="M36" t="s">
-        <v>32</v>
-      </c>
-      <c r="N36" s="7" t="s">
-        <v>380</v>
-      </c>
-      <c r="O36" s="7" t="s">
-        <v>381</v>
+        <v>102</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>382</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>44397.036516203705</v>
+      </c>
       <c r="B37" s="2" t="s">
-        <v>383</v>
+        <v>127</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>384</v>
+        <v>128</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>385</v>
+        <v>129</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>359</v>
+        <v>99</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>396</v>
+        <v>130</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>66</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="I37" s="2"/>
       <c r="J37" s="2" t="s">
-        <v>386</v>
+        <v>45</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>387</v>
+        <v>131</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>388</v>
+        <v>41</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="N37" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="O37" s="7" t="s">
-        <v>390</v>
+        <v>26</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>391</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>44411.776064814818</v>
+      </c>
       <c r="B38" s="2" t="s">
-        <v>392</v>
+        <v>161</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>393</v>
+        <v>162</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="E38" t="s">
-        <v>359</v>
+        <v>163</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>395</v>
+        <v>164</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>398</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="I38" s="2"/>
       <c r="J38" s="2" t="s">
-        <v>399</v>
+        <v>165</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>31</v>
+        <v>242</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>400</v>
+        <v>41</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="N38" s="7" t="s">
-        <v>401</v>
-      </c>
-      <c r="O38" s="7" t="s">
-        <v>402</v>
+        <v>126</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>403</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>404</v>
+        <v>423</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>405</v>
+        <v>162</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="E39" t="s">
+        <v>424</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>359</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>407</v>
+        <v>425</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="I39" s="2"/>
+        <v>426</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>369</v>
+      </c>
       <c r="J39" s="2" t="s">
-        <v>408</v>
+        <v>427</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>409</v>
+        <v>428</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="N39" s="7" t="s">
-        <v>410</v>
+        <v>429</v>
       </c>
       <c r="O39" s="7" t="s">
-        <v>411</v>
+        <v>430</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>412</v>
+        <v>431</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>44405.648368055554</v>
+      </c>
       <c r="B40" s="2" t="s">
-        <v>413</v>
+        <v>203</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>357</v>
+        <v>204</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>414</v>
+        <v>205</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>359</v>
+        <v>99</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>415</v>
+        <v>206</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>267</v>
+        <v>35</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>416</v>
+        <v>138</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>417</v>
+        <v>207</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>418</v>
+        <v>208</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>419</v>
+        <v>209</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N40" s="7" t="s">
-        <v>420</v>
-      </c>
-      <c r="O40" s="7" t="s">
-        <v>421</v>
+        <v>46</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>422</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>44396.946180555555</v>
+      </c>
       <c r="B41" s="2" t="s">
-        <v>423</v>
+        <v>169</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>424</v>
+        <v>171</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>359</v>
+        <v>99</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>425</v>
+        <v>38</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>369</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="I41" s="2"/>
       <c r="J41" s="2" t="s">
-        <v>427</v>
+        <v>173</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>31</v>
+        <v>174</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>428</v>
+        <v>175</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N41" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="O41" s="7" t="s">
-        <v>430</v>
+        <v>32</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>431</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P33">
-    <sortCondition ref="C2:C33"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P41">
+    <sortCondition ref="C2:C41"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="O13" r:id="rId1" xr:uid="{9E307C65-887C-5044-8DB8-E71EB3F10045}"/>
-    <hyperlink ref="O7" r:id="rId2" xr:uid="{4A81FE9A-EBAB-0747-B2F3-61D7490B1D68}"/>
-    <hyperlink ref="O11" r:id="rId3" xr:uid="{448DA057-37C3-3B4D-9D30-C27C2FD902D3}"/>
-    <hyperlink ref="O14" r:id="rId4" xr:uid="{85DCA030-31D8-4740-B777-FBA97285460E}"/>
-    <hyperlink ref="O18" r:id="rId5" xr:uid="{5A40EFE8-502D-2149-ACBE-311EA5579DF3}"/>
-    <hyperlink ref="O10" r:id="rId6" xr:uid="{7E0B92DD-CBCC-8F46-B940-A199BDE9BF18}"/>
-    <hyperlink ref="O17" r:id="rId7" xr:uid="{6A6E0364-629D-FF44-817A-6C9F4E3C32C0}"/>
-    <hyperlink ref="O21" r:id="rId8" xr:uid="{7DAAB33D-9347-8F48-A5B6-88CA9022F3F4}"/>
-    <hyperlink ref="N6" r:id="rId9" xr:uid="{3FEE33F3-63FD-49C4-92AB-1042A2591AA6}"/>
-    <hyperlink ref="O6" r:id="rId10" xr:uid="{7CBE67B6-B9B5-45EE-9470-F4AA5E5FF358}"/>
-    <hyperlink ref="N34" r:id="rId11" xr:uid="{7712592D-C212-4A93-BA25-D4658CFA663A}"/>
-    <hyperlink ref="O34" r:id="rId12" xr:uid="{E70F50EC-A19F-4DA1-9215-7A17F732F801}"/>
-    <hyperlink ref="N35" r:id="rId13" xr:uid="{56DE9EB8-7714-4395-9CD4-AF9B7F618754}"/>
-    <hyperlink ref="O35" r:id="rId14" xr:uid="{C79E0D61-6BF8-4D23-9016-8FA43E7BA486}"/>
-    <hyperlink ref="N36" r:id="rId15" xr:uid="{5B38EE64-6D4D-430D-9621-00ED2C8B8D7A}"/>
-    <hyperlink ref="O36" r:id="rId16" xr:uid="{01DBDDE2-32E1-4266-A6A7-FDED7088E189}"/>
-    <hyperlink ref="N37" r:id="rId17" xr:uid="{D7196034-9BFC-401F-8AD8-444A5A8F0488}"/>
-    <hyperlink ref="O37" r:id="rId18" xr:uid="{EBB06DFB-D7BE-4833-AFA8-B29F5EB78FCE}"/>
-    <hyperlink ref="N38" r:id="rId19" xr:uid="{75085428-AD2A-4222-ACFA-ED2B329717F2}"/>
-    <hyperlink ref="O38" r:id="rId20" xr:uid="{8AD637F9-AD2E-42B3-9D8D-76C11471058D}"/>
-    <hyperlink ref="N39" r:id="rId21" xr:uid="{120B96FF-057F-4C8A-B466-35389F9A4CD8}"/>
-    <hyperlink ref="O39" r:id="rId22" xr:uid="{BC0B539C-D47A-4142-91C2-D1991320DA6E}"/>
-    <hyperlink ref="N40" r:id="rId23" xr:uid="{B153E7EE-184D-4F41-8EAC-022CA1AFC245}"/>
-    <hyperlink ref="O40" r:id="rId24" xr:uid="{53635958-96CA-44CA-B081-1F20CB88B225}"/>
-    <hyperlink ref="N41" r:id="rId25" xr:uid="{BC598059-63C8-462E-852A-A0B1E342929A}"/>
-    <hyperlink ref="O41" r:id="rId26" xr:uid="{31B14771-D13B-4480-85D7-DFC9490D3475}"/>
+    <hyperlink ref="O18" r:id="rId1" xr:uid="{9E307C65-887C-5044-8DB8-E71EB3F10045}"/>
+    <hyperlink ref="O12" r:id="rId2" xr:uid="{4A81FE9A-EBAB-0747-B2F3-61D7490B1D68}"/>
+    <hyperlink ref="O16" r:id="rId3" xr:uid="{448DA057-37C3-3B4D-9D30-C27C2FD902D3}"/>
+    <hyperlink ref="O20" r:id="rId4" xr:uid="{85DCA030-31D8-4740-B777-FBA97285460E}"/>
+    <hyperlink ref="O24" r:id="rId5" xr:uid="{5A40EFE8-502D-2149-ACBE-311EA5579DF3}"/>
+    <hyperlink ref="O15" r:id="rId6" xr:uid="{7E0B92DD-CBCC-8F46-B940-A199BDE9BF18}"/>
+    <hyperlink ref="O23" r:id="rId7" xr:uid="{6A6E0364-629D-FF44-817A-6C9F4E3C32C0}"/>
+    <hyperlink ref="O27" r:id="rId8" xr:uid="{7DAAB33D-9347-8F48-A5B6-88CA9022F3F4}"/>
+    <hyperlink ref="N10" r:id="rId9" xr:uid="{3FEE33F3-63FD-49C4-92AB-1042A2591AA6}"/>
+    <hyperlink ref="O10" r:id="rId10" xr:uid="{7CBE67B6-B9B5-45EE-9470-F4AA5E5FF358}"/>
+    <hyperlink ref="N6" r:id="rId11" xr:uid="{7712592D-C212-4A93-BA25-D4658CFA663A}"/>
+    <hyperlink ref="O6" r:id="rId12" xr:uid="{E70F50EC-A19F-4DA1-9215-7A17F732F801}"/>
+    <hyperlink ref="N34" r:id="rId13" xr:uid="{56DE9EB8-7714-4395-9CD4-AF9B7F618754}"/>
+    <hyperlink ref="O34" r:id="rId14" xr:uid="{C79E0D61-6BF8-4D23-9016-8FA43E7BA486}"/>
+    <hyperlink ref="N8" r:id="rId15" xr:uid="{5B38EE64-6D4D-430D-9621-00ED2C8B8D7A}"/>
+    <hyperlink ref="O8" r:id="rId16" xr:uid="{01DBDDE2-32E1-4266-A6A7-FDED7088E189}"/>
+    <hyperlink ref="N3" r:id="rId17" xr:uid="{D7196034-9BFC-401F-8AD8-444A5A8F0488}"/>
+    <hyperlink ref="O3" r:id="rId18" xr:uid="{EBB06DFB-D7BE-4833-AFA8-B29F5EB78FCE}"/>
+    <hyperlink ref="N19" r:id="rId19" xr:uid="{75085428-AD2A-4222-ACFA-ED2B329717F2}"/>
+    <hyperlink ref="O19" r:id="rId20" xr:uid="{8AD637F9-AD2E-42B3-9D8D-76C11471058D}"/>
+    <hyperlink ref="N11" r:id="rId21" xr:uid="{120B96FF-057F-4C8A-B466-35389F9A4CD8}"/>
+    <hyperlink ref="O11" r:id="rId22" xr:uid="{BC0B539C-D47A-4142-91C2-D1991320DA6E}"/>
+    <hyperlink ref="N7" r:id="rId23" xr:uid="{B153E7EE-184D-4F41-8EAC-022CA1AFC245}"/>
+    <hyperlink ref="O7" r:id="rId24" xr:uid="{53635958-96CA-44CA-B081-1F20CB88B225}"/>
+    <hyperlink ref="N39" r:id="rId25" xr:uid="{BC598059-63C8-462E-852A-A0B1E342929A}"/>
+    <hyperlink ref="O39" r:id="rId26" xr:uid="{31B14771-D13B-4480-85D7-DFC9490D3475}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId27"/>

</xml_diff>

<commit_message>
fam trees additions + edit requests
</commit_message>
<xml_diff>
--- a/src/data/summer21/bios_summer21.xlsx
+++ b/src/data/summer21/bios_summer21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorin\dspuci-website-gatsby\src\data\summer21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BDEFA0-E954-4FB0-BC56-42994B1ED81D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ABB6A6-D3C3-4BB8-8818-82B90075CAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10176" yWindow="1848" windowWidth="12960" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="430">
   <si>
     <t>Timestamp</t>
   </si>
@@ -511,9 +511,6 @@
     <t>Castro Valley, CA</t>
   </si>
   <si>
-    <t>Finance, Consulting, Human Resources</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/jennyywuu/</t>
   </si>
   <si>
@@ -731,9 +728,6 @@
   </si>
   <si>
     <t>Psychological Science</t>
-  </si>
-  <si>
-    <t>HRMA , Student Assistant at Paul Merage, MUSA Representative (2019-2020)</t>
   </si>
   <si>
     <t xml:space="preserve">Hi! My name is Tiffany Than and I initiated in my fall quarter of my first year here at UCI in 2019. In my free time I enjoy exploring new eateries, making Spotify playlists, and seeing live concerts! A fun fact about myself is that I named my car Adeline. Ask me about music/tv shows, my thoughts on mukbangs, or anything at recruitment! 
@@ -743,9 +737,6 @@
     <t>Literary Journalism, Information and Computer Science</t>
   </si>
   <si>
-    <t>Recruitment + Retention Intern at ASUCI</t>
-  </si>
-  <si>
     <t>Tommy</t>
   </si>
   <si>
@@ -800,9 +791,6 @@
     <t>Social Media Intern at J.ING</t>
   </si>
   <si>
-    <t>HR Business Partner, Global Online Intern at The Estee Lauder Companies</t>
-  </si>
-  <si>
     <t>Nathan</t>
   </si>
   <si>
@@ -887,18 +875,12 @@
     <t>Portland, OR</t>
   </si>
   <si>
-    <t>Consulting, Real Estate, Human Resources</t>
-  </si>
-  <si>
     <t>MUSA Representatives</t>
   </si>
   <si>
     <t>julialin@ucidsp.com</t>
   </si>
   <si>
-    <t>Hi hi hi! My name is Julia Lin and I initiated in the fall quarter of my Freshman year with the Alpha Mu class. In my free time, I like to read, travel, and find new shows/movies to watch. Some fun facts about me are that I have my own Lululemon e-commerce business, I've never had a marshmallow before, and I'm also a Canadian Dual-Citizen! Feel free to ask me about anything at recruitment whether it's about the favorite places I've traveled to or about my dog Princess :-)</t>
-  </si>
-  <si>
     <t>Jake</t>
   </si>
   <si>
@@ -1028,12 +1010,6 @@
     <t>Anthropology, Digital Information Systems</t>
   </si>
   <si>
-    <t>Digital Marketing Intern at Coronado Shores Company</t>
-  </si>
-  <si>
-    <t>MUSA Representatives, ASUCI, Campus Representatives</t>
-  </si>
-  <si>
     <t>MUSA, Product Association, Previous: AMP Mentee</t>
   </si>
   <si>
@@ -1317,6 +1293,24 @@
   </si>
   <si>
     <t>Software Developer at LinQuest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finance/Business Operations Acquisition Intern at NASA Jet Propulsion Laboratory </t>
+  </si>
+  <si>
+    <t>Amazon Prime Campus Ambassador, Campus Representatives, Red Bull Student Marketeer</t>
+  </si>
+  <si>
+    <t>Hi! My name is Julia and I initiated in the fall of my freshman year with the Alpha Mu class. Some fun facts about me are that I’m a little bit of a shopaholic and that you might see me around campus giving tours since I’m a tour guide for UCI. Ask me about my favorite flavor of Red Bull or anything at recruitment :-)</t>
+  </si>
+  <si>
+    <t>Change Management Operations Intern at PayPal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HRMA, Student Assistant at Paul Merage Specialty Masters Program, MUSA Representative </t>
+  </si>
+  <si>
+    <t>HR Intern at Kaiser Permanente</t>
   </si>
 </sst>
 </file>
@@ -1398,7 +1392,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1413,6 +1407,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1735,10 +1732,10 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="P26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1838,7 +1835,7 @@
         <v>147</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>31</v>
@@ -1858,22 +1855,22 @@
     </row>
     <row r="3" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>35</v>
@@ -1882,25 +1879,25 @@
         <v>66</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>68</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -1914,7 +1911,7 @@
         <v>64</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -1932,13 +1929,13 @@
         <v>66</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>214</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>48</v>
@@ -1950,7 +1947,7 @@
         <v>86</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -1958,13 +1955,13 @@
         <v>44404.857893518521</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>99</v>
@@ -1980,39 +1977,39 @@
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="N5" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>40</v>
@@ -2024,89 +2021,89 @@
         <v>51</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>17</v>
@@ -2121,25 +2118,25 @@
         <v>66</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="M8" t="s">
         <v>32</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -2147,13 +2144,13 @@
         <v>44404.653217592589</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>228</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>123</v>
@@ -2162,7 +2159,7 @@
         <v>40</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>44</v>
@@ -2172,22 +2169,22 @@
         <v>45</v>
       </c>
       <c r="K9" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>231</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>50</v>
       </c>
       <c r="N9" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="O9" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="P9" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -2195,108 +2192,108 @@
         <v>44397.382604166669</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>51</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="E11" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>23</v>
@@ -2311,25 +2308,25 @@
         <v>66</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>46</v>
       </c>
       <c r="N12" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2387,13 +2384,13 @@
         <v>44397.802523148152</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>99</v>
@@ -2409,10 +2406,10 @@
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>41</v>
@@ -2421,39 +2418,39 @@
         <v>58</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>31</v>
@@ -2465,57 +2462,57 @@
         <v>20</v>
       </c>
       <c r="N15" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>50</v>
       </c>
       <c r="N16" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="O16" s="7" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -2523,13 +2520,13 @@
         <v>44398.992349537039</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>123</v>
@@ -2544,169 +2541,169 @@
         <v>35</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K17" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>125</v>
       </c>
       <c r="N17" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="O17" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="P17" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>66</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>46</v>
       </c>
       <c r="N18" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="E19" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>48</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>288</v>
+        <v>100</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>335</v>
+        <v>424</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>336</v>
+        <v>425</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>46</v>
       </c>
       <c r="N20" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="O20" s="7" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>291</v>
+        <v>426</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -2720,7 +2717,7 @@
         <v>60</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>16</v>
@@ -2741,10 +2738,10 @@
         <v>30</v>
       </c>
       <c r="K21" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L21" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>50</v>
@@ -2756,7 +2753,7 @@
         <v>87</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -2770,7 +2767,7 @@
         <v>78</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>42</v>
@@ -2785,13 +2782,13 @@
         <v>24</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>80</v>
@@ -2811,22 +2808,22 @@
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>35</v>
@@ -2835,36 +2832,36 @@
         <v>147</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>58</v>
       </c>
       <c r="N23" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>17</v>
@@ -2876,25 +2873,25 @@
         <v>24</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N24" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2927,7 +2924,7 @@
         <v>30</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>113</v>
@@ -2974,10 +2971,10 @@
         <v>118</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>119</v>
@@ -2997,22 +2994,22 @@
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>24</v>
@@ -3024,22 +3021,22 @@
         <v>100</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>48</v>
       </c>
       <c r="N27" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3119,10 +3116,10 @@
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>31</v>
@@ -3137,7 +3134,7 @@
         <v>155</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3151,7 +3148,7 @@
         <v>75</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>16</v>
@@ -3166,16 +3163,16 @@
         <v>24</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>57</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>259</v>
+        <v>427</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>237</v>
+        <v>428</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>26</v>
@@ -3186,8 +3183,8 @@
       <c r="O30" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="P30" s="2" t="s">
-        <v>238</v>
+      <c r="P30" s="11" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3225,7 +3222,7 @@
         <v>158</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>46</v>
@@ -3237,7 +3234,7 @@
         <v>92</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3251,7 +3248,7 @@
         <v>83</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>16</v>
@@ -3267,13 +3264,13 @@
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="K32" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="L32" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>224</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>58</v>
@@ -3285,7 +3282,7 @@
         <v>93</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3293,13 +3290,13 @@
         <v>44404.80846064815</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>123</v>
@@ -3308,48 +3305,48 @@
         <v>23</v>
       </c>
       <c r="G33" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="J33" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="K33" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="I33" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>248</v>
-      </c>
       <c r="L33" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>36</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>40</v>
@@ -3361,13 +3358,13 @@
         <v>35</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>31</v>
@@ -3376,13 +3373,13 @@
         <v>48</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="O34" s="7" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3396,7 +3393,7 @@
         <v>37</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>16</v>
@@ -3405,7 +3402,7 @@
         <v>23</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>35</v>
@@ -3415,10 +3412,10 @@
         <v>25</v>
       </c>
       <c r="K35" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="L35" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>219</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>26</v>
@@ -3430,7 +3427,7 @@
         <v>94</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3459,7 +3456,7 @@
         <v>24</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>100</v>
@@ -3513,7 +3510,7 @@
         <v>45</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>41</v>
@@ -3558,10 +3555,10 @@
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2" t="s">
-        <v>163</v>
+        <v>57</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>240</v>
+        <v>429</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>41</v>
@@ -3570,60 +3567,60 @@
         <v>125</v>
       </c>
       <c r="N38" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="O38" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="O38" s="2" t="s">
+      <c r="P38" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="P38" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>160</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="N39" s="7" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="O39" s="7" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3631,13 +3628,13 @@
         <v>44405.648368055554</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>99</v>
@@ -3646,7 +3643,7 @@
         <v>40</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>35</v>
@@ -3655,25 +3652,25 @@
         <v>136</v>
       </c>
       <c r="J40" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="K40" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="K40" s="2" t="s">
+      <c r="L40" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>46</v>
       </c>
       <c r="N40" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="O40" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="O40" s="2" t="s">
+      <c r="P40" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="P40" s="2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3681,13 +3678,13 @@
         <v>44396.946180555555</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>99</v>
@@ -3699,29 +3696,29 @@
         <v>38</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="K41" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="K41" s="2" t="s">
+      <c r="L41" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N41" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="O41" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="O41" s="2" t="s">
+      <c r="P41" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="P41" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added bro info + chen-ho
</commit_message>
<xml_diff>
--- a/src/data/summer21/bios_summer21.xlsx
+++ b/src/data/summer21/bios_summer21.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorin\dspuci-website-gatsby\src\data\summer21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorin\newest_dspuci_website\dspuci-website-gatsby\src\data\summer21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ABB6A6-D3C3-4BB8-8818-82B90075CAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3AF416-86CE-466E-B94B-1ACCE701EEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10176" yWindow="1848" windowWidth="12960" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7788" yWindow="60" windowWidth="12960" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="433">
   <si>
     <t>Timestamp</t>
   </si>
@@ -571,15 +571,6 @@
     <t>kelsie_kim</t>
   </si>
   <si>
-    <t>Public Health, Management</t>
-  </si>
-  <si>
-    <t>Marketing Administrative Assistant at DPM Link</t>
-  </si>
-  <si>
-    <t>Marketing Association</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/kelsiek52/</t>
   </si>
   <si>
@@ -707,12 +698,6 @@
   </si>
   <si>
     <t>Koenigstein im Taunus, Germany</t>
-  </si>
-  <si>
-    <t>Data Science Intern at IQVIA</t>
-  </si>
-  <si>
-    <t>Association for Computing Machinery, STAIRS Lab</t>
   </si>
   <si>
     <t>https://www.linkedin.com/in/devine-sean/</t>
@@ -890,18 +875,9 @@
     <t>jake_moss</t>
   </si>
   <si>
-    <t>Real Estate Finance, Product Management</t>
-  </si>
-  <si>
-    <t>MUSA</t>
-  </si>
-  <si>
     <t>jakemoss@ucidsp.com</t>
   </si>
   <si>
-    <t>Hi!! My name is Jake and I initiated in the fall of my freshman year with the Alpha Mu class. In my free time, I enjoy surfing, fishing, golfing, playing tennis, and listening to music. A fun fact about myself is that I accidentally lit my couch on fire. Ask me about my favorite comedians, Netflix/tv shows, or anything at recruitment!</t>
-  </si>
-  <si>
     <t>Jason</t>
   </si>
   <si>
@@ -953,15 +929,9 @@
     <t>San Francisco, CA</t>
   </si>
   <si>
-    <t>Launch@Apple Mentee</t>
-  </si>
-  <si>
     <t>winnieqi@ucidsp.com</t>
   </si>
   <si>
-    <t>Hello!!! My name is Winnie and I initiated fall quarter of my second year with the Alpha Mu class. In my free time, I like to play basketball, curate Spotify playlists, and try new food spots. A fun fact about me is that I grew 5 inches in a span of one summer. Ask me about my favorite TV shows, artists, food cuisines, or anything at recruitment :))</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/nathan-lee1/</t>
   </si>
   <si>
@@ -1311,6 +1281,45 @@
   </si>
   <si>
     <t>HR Intern at Kaiser Permanente</t>
+  </si>
+  <si>
+    <t>Finance Extern at Apple; Client Group Intern at Wellington</t>
+  </si>
+  <si>
+    <t>Hi!! My name is Winnie and I initiated fall quarter of my second year with the Alpha Mu class. In my free time, I love playing basketball, trying new food spots, hammocking in Aldrich, and binge-watching architectural digest vids! Fun fact I've made 218+ Spotify playlists over the years! See you at recruitment :)</t>
+  </si>
+  <si>
+    <t>Software Engineering, Finance</t>
+  </si>
+  <si>
+    <t>Software Engineering Intern at Duck Creek Technologies</t>
+  </si>
+  <si>
+    <t>Association for Computing Machinery</t>
+  </si>
+  <si>
+    <t>Public Health &amp; Management</t>
+  </si>
+  <si>
+    <t>Universal Pictures CampusU Marketing Representative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAISS, President of Marketing Association ('21-'22) </t>
+  </si>
+  <si>
+    <t>Digital Information Systems, Spanish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finance, Product Management </t>
+  </si>
+  <si>
+    <t>Product Development Intern at Billabong</t>
+  </si>
+  <si>
+    <t>MUSA; Associate</t>
+  </si>
+  <si>
+    <t>Hi! My name is Jake and I initiated in the fall of my freshman year with the Alpha Mu class. In my free time I enjoy surfing, playing tennis and listening to music. Ask me about my favorite comedians, or anything at recruitment!</t>
   </si>
 </sst>
 </file>
@@ -1732,10 +1741,10 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1835,7 +1844,7 @@
         <v>147</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>31</v>
@@ -1855,22 +1864,22 @@
     </row>
     <row r="3" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>35</v>
@@ -1879,25 +1888,25 @@
         <v>66</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>68</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -1911,7 +1920,7 @@
         <v>64</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -1929,13 +1938,13 @@
         <v>66</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>48</v>
@@ -1947,7 +1956,7 @@
         <v>86</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -1955,13 +1964,13 @@
         <v>44404.857893518521</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>99</v>
@@ -1977,39 +1986,39 @@
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>40</v>
@@ -2021,89 +2030,89 @@
         <v>51</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>17</v>
@@ -2118,25 +2127,25 @@
         <v>66</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="M8" t="s">
         <v>32</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -2144,13 +2153,13 @@
         <v>44404.653217592589</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>123</v>
@@ -2159,32 +2168,32 @@
         <v>40</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>44</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>45</v>
+        <v>422</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>229</v>
+        <v>423</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>230</v>
+        <v>424</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>50</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -2192,108 +2201,108 @@
         <v>44397.382604166669</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>51</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="E11" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>23</v>
@@ -2308,25 +2317,25 @@
         <v>66</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>46</v>
       </c>
       <c r="N12" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2384,13 +2393,13 @@
         <v>44397.802523148152</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>99</v>
@@ -2406,10 +2415,10 @@
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>41</v>
@@ -2418,39 +2427,39 @@
         <v>58</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>31</v>
@@ -2462,57 +2471,57 @@
         <v>20</v>
       </c>
       <c r="N15" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>50</v>
       </c>
       <c r="N16" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="O16" s="7" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -2541,169 +2550,169 @@
         <v>35</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>183</v>
+        <v>425</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>184</v>
+        <v>426</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>185</v>
+        <v>427</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>125</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>66</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>46</v>
       </c>
       <c r="N18" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="E19" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>48</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>46</v>
       </c>
       <c r="N20" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="O20" s="7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -2767,7 +2776,7 @@
         <v>78</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>42</v>
@@ -2782,13 +2791,13 @@
         <v>24</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>80</v>
@@ -2808,22 +2817,22 @@
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>35</v>
@@ -2832,36 +2841,36 @@
         <v>147</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>58</v>
       </c>
       <c r="N23" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>17</v>
@@ -2872,26 +2881,29 @@
       <c r="H24" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="I24" s="2" t="s">
+        <v>428</v>
+      </c>
       <c r="J24" s="2" t="s">
-        <v>289</v>
+        <v>429</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>31</v>
+        <v>430</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>290</v>
+        <v>431</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N24" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>292</v>
+        <v>432</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2924,7 +2936,7 @@
         <v>30</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>113</v>
@@ -2971,10 +2983,10 @@
         <v>118</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>119</v>
@@ -2994,49 +3006,47 @@
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="I27" s="2"/>
       <c r="J27" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>310</v>
+        <v>420</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>48</v>
       </c>
       <c r="N27" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>312</v>
+        <v>421</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3116,10 +3126,10 @@
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>31</v>
@@ -3134,7 +3144,7 @@
         <v>155</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3148,7 +3158,7 @@
         <v>75</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>16</v>
@@ -3163,16 +3173,16 @@
         <v>24</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>57</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>26</v>
@@ -3184,7 +3194,7 @@
         <v>91</v>
       </c>
       <c r="P30" s="11" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3222,7 +3232,7 @@
         <v>158</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>46</v>
@@ -3234,7 +3244,7 @@
         <v>92</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3248,7 +3258,7 @@
         <v>83</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>16</v>
@@ -3264,13 +3274,13 @@
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>58</v>
@@ -3282,7 +3292,7 @@
         <v>93</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3290,13 +3300,13 @@
         <v>44404.80846064815</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>123</v>
@@ -3305,48 +3315,48 @@
         <v>23</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>36</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>40</v>
@@ -3358,13 +3368,13 @@
         <v>35</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>31</v>
@@ -3373,13 +3383,13 @@
         <v>48</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="O34" s="7" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3393,7 +3403,7 @@
         <v>37</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>16</v>
@@ -3402,7 +3412,7 @@
         <v>23</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>35</v>
@@ -3412,10 +3422,10 @@
         <v>25</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>26</v>
@@ -3427,7 +3437,7 @@
         <v>94</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3456,7 +3466,7 @@
         <v>24</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>100</v>
@@ -3510,7 +3520,7 @@
         <v>45</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>41</v>
@@ -3558,7 +3568,7 @@
         <v>57</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>41</v>
@@ -3578,49 +3588,49 @@
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>160</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="N39" s="7" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="O39" s="7" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3628,13 +3638,13 @@
         <v>44405.648368055554</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>99</v>
@@ -3643,7 +3653,7 @@
         <v>40</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>35</v>
@@ -3652,25 +3662,25 @@
         <v>136</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>46</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added alex's stats minor
</commit_message>
<xml_diff>
--- a/src/data/summer21/bios_summer21.xlsx
+++ b/src/data/summer21/bios_summer21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorin\newest_dspuci_website\dspuci-website-gatsby\src\data\summer21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0E2EAF-A298-4B64-8805-FED7CA3C8793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F879FCD-2A84-4A39-AE56-3EA70A20D0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7788" yWindow="60" windowWidth="12960" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -352,9 +352,6 @@
     <t>alex_pham</t>
   </si>
   <si>
-    <t>Philosophy</t>
-  </si>
-  <si>
     <t>MAISS, Product Association @ UCI</t>
   </si>
   <si>
@@ -1290,6 +1287,9 @@
   </si>
   <si>
     <t>Finance, Accounting, Real Estate</t>
+  </si>
+  <si>
+    <t>Philosophy, Statistics</t>
   </si>
 </sst>
 </file>
@@ -1711,10 +1711,10 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
+      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1789,32 +1789,32 @@
         <v>44404.516250000001</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>35</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>31</v>
@@ -1823,33 +1823,33 @@
         <v>67</v>
       </c>
       <c r="N2" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>349</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>35</v>
@@ -1858,25 +1858,25 @@
         <v>65</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>351</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>352</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>67</v>
       </c>
       <c r="N3" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="O3" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="P3" s="2" t="s">
         <v>354</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -1890,7 +1890,7 @@
         <v>63</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -1908,13 +1908,13 @@
         <v>65</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>418</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>419</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>47</v>
@@ -1926,7 +1926,7 @@
         <v>79</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -1934,13 +1934,13 @@
         <v>44404.857893518521</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>91</v>
@@ -1956,39 +1956,39 @@
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="N5" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>323</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>40</v>
@@ -2000,89 +2000,89 @@
         <v>50</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>329</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N6" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="O6" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="O6" s="7" t="s">
-        <v>327</v>
-      </c>
       <c r="P6" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>378</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>382</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>383</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N7" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="O7" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="P7" s="2" t="s">
         <v>385</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>341</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>17</v>
@@ -2097,25 +2097,25 @@
         <v>65</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M8" t="s">
         <v>32</v>
       </c>
       <c r="N8" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="O8" s="7" t="s">
         <v>344</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="P8" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -2123,47 +2123,47 @@
         <v>44404.653217592589</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>211</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>409</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>49</v>
       </c>
       <c r="N9" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="O9" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="P9" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -2171,108 +2171,108 @@
         <v>44397.382604166669</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>299</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>50</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N10" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="O10" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="O10" s="7" t="s">
-        <v>301</v>
-      </c>
       <c r="P10" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>370</v>
-      </c>
       <c r="E11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N11" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="O11" s="7" t="s">
         <v>374</v>
       </c>
-      <c r="O11" s="7" t="s">
+      <c r="P11" s="2" t="s">
         <v>375</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>248</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>23</v>
@@ -2287,25 +2287,25 @@
         <v>65</v>
       </c>
       <c r="J12" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>45</v>
       </c>
       <c r="N12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O12" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="P12" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2313,13 +2313,13 @@
         <v>44396.99622685185</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>91</v>
@@ -2328,34 +2328,34 @@
         <v>23</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="L13" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N13" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="O13" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="P13" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -2363,13 +2363,13 @@
         <v>44397.802523148152</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>91</v>
@@ -2385,10 +2385,10 @@
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>41</v>
@@ -2397,39 +2397,39 @@
         <v>57</v>
       </c>
       <c r="N14" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="O14" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="O14" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="P14" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>273</v>
-      </c>
       <c r="E15" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>31</v>
@@ -2441,57 +2441,57 @@
         <v>20</v>
       </c>
       <c r="N15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="O15" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>256</v>
-      </c>
       <c r="E16" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>49</v>
       </c>
       <c r="N16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="O16" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="P16" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -2499,16 +2499,16 @@
         <v>44398.992349537039</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>23</v>
@@ -2520,169 +2520,169 @@
         <v>35</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K17" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="L17" s="2" t="s">
-        <v>412</v>
-      </c>
       <c r="M17" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N17" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="O17" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="P17" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G18" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>65</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K18" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="L18" s="10" t="s">
         <v>309</v>
-      </c>
-      <c r="L18" s="10" t="s">
-        <v>310</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>45</v>
       </c>
       <c r="N18" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>358</v>
-      </c>
       <c r="E19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H19" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="J19" s="2" t="s">
         <v>362</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>363</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N19" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="O19" s="7" t="s">
         <v>365</v>
       </c>
-      <c r="O19" s="7" t="s">
+      <c r="P19" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>263</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>92</v>
       </c>
       <c r="K20" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>399</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>400</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>45</v>
       </c>
       <c r="N20" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O20" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -2696,7 +2696,7 @@
         <v>59</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>16</v>
@@ -2717,10 +2717,10 @@
         <v>30</v>
       </c>
       <c r="K21" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="L21" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>49</v>
@@ -2732,98 +2732,98 @@
         <v>80</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>35</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K22" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="L22" s="2" t="s">
         <v>314</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>315</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>57</v>
       </c>
       <c r="N22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="O22" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>269</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I23" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="K23" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="L23" s="2" t="s">
         <v>415</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>416</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2856,7 +2856,7 @@
         <v>30</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>105</v>
@@ -2900,48 +2900,48 @@
         <v>51</v>
       </c>
       <c r="I25" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="L25" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N25" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="O25" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="O25" s="2" t="s">
+      <c r="P25" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>286</v>
-      </c>
       <c r="E26" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>24</v>
@@ -2951,22 +2951,22 @@
         <v>92</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="O26" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3024,16 +3024,16 @@
         <v>44409.99291666667</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="E28" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>40</v>
@@ -3046,10 +3046,10 @@
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>31</v>
@@ -3058,13 +3058,13 @@
         <v>67</v>
       </c>
       <c r="N28" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="O28" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="O28" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="P28" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3078,7 +3078,7 @@
         <v>74</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>16</v>
@@ -3093,16 +3093,16 @@
         <v>24</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>56</v>
       </c>
       <c r="K29" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="L29" s="2" t="s">
         <v>402</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>403</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>26</v>
@@ -3114,7 +3114,7 @@
         <v>83</v>
       </c>
       <c r="P29" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3128,7 +3128,7 @@
         <v>53</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>16</v>
@@ -3146,13 +3146,13 @@
         <v>54</v>
       </c>
       <c r="J30" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="K30" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="L30" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>45</v>
@@ -3164,7 +3164,7 @@
         <v>84</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3178,7 +3178,7 @@
         <v>76</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>16</v>
@@ -3194,13 +3194,13 @@
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="K31" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="L31" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>57</v>
@@ -3212,7 +3212,7 @@
         <v>85</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3220,63 +3220,63 @@
         <v>44404.80846064815</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="E32" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G32" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="J32" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="K32" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="K32" s="2" t="s">
-        <v>227</v>
-      </c>
       <c r="L32" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>36</v>
       </c>
       <c r="N32" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="O32" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="O32" s="2" t="s">
+      <c r="P32" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="P32" s="2" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>332</v>
-      </c>
       <c r="E33" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>40</v>
@@ -3288,13 +3288,13 @@
         <v>35</v>
       </c>
       <c r="I33" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="J33" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="K33" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>31</v>
@@ -3303,13 +3303,13 @@
         <v>47</v>
       </c>
       <c r="N33" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="O33" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="O33" s="7" t="s">
-        <v>338</v>
-      </c>
       <c r="P33" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3323,7 +3323,7 @@
         <v>37</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>16</v>
@@ -3332,7 +3332,7 @@
         <v>23</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>35</v>
@@ -3342,10 +3342,10 @@
         <v>25</v>
       </c>
       <c r="K34" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="L34" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>26</v>
@@ -3357,7 +3357,7 @@
         <v>86</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3386,7 +3386,7 @@
         <v>24</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>92</v>
@@ -3415,13 +3415,13 @@
         <v>44397.036516203705</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>91</v>
@@ -3430,7 +3430,7 @@
         <v>40</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>43</v>
@@ -3440,7 +3440,7 @@
         <v>44</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>41</v>
@@ -3449,13 +3449,13 @@
         <v>26</v>
       </c>
       <c r="N36" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="O36" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="O36" s="2" t="s">
+      <c r="P36" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="P36" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3463,22 +3463,22 @@
         <v>44411.776064814818</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="E37" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>24</v>
@@ -3488,69 +3488,69 @@
         <v>56</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>41</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N37" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="O37" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="O37" s="2" t="s">
+      <c r="P37" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>388</v>
-      </c>
       <c r="E38" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G38" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="I38" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="L38" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>391</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>36</v>
       </c>
       <c r="N38" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="O38" s="7" t="s">
         <v>392</v>
       </c>
-      <c r="O38" s="7" t="s">
+      <c r="P38" s="2" t="s">
         <v>393</v>
-      </c>
-      <c r="P38" s="2" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3558,13 +3558,13 @@
         <v>44405.648368055554</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>91</v>
@@ -3573,34 +3573,34 @@
         <v>40</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>35</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J39" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="K39" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="K39" s="2" t="s">
+      <c r="L39" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>45</v>
       </c>
       <c r="N39" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="O39" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="O39" s="2" t="s">
+      <c r="P39" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="P39" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3608,13 +3608,13 @@
         <v>44396.946180555555</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>91</v>
@@ -3626,29 +3626,29 @@
         <v>38</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="K40" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K40" s="2" t="s">
+      <c r="L40" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N40" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="O40" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="O40" s="2" t="s">
+      <c r="P40" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="P40" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Dylan's Photo & Jacob's bio
</commit_message>
<xml_diff>
--- a/src/data/summer21/bios_summer21.xlsx
+++ b/src/data/summer21/bios_summer21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\kcow\code\dspuci-website-gatsby\src\data\summer21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E707405-F49F-4DB4-9FCB-0097476D9A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF187C7-E47D-4BEE-9C11-F78986EB3F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4890" yWindow="1935" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -1331,12 +1331,6 @@
     <t>Fullerton, CA</t>
   </si>
   <si>
-    <t>Marketing, Consulting</t>
-  </si>
-  <si>
-    <t>BCEC</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/jacobwon/</t>
   </si>
   <si>
@@ -1512,6 +1506,12 @@
   </si>
   <si>
     <t>Hi everyone! My name is Maryam and I initiated in Fall of ‘22 with the Alpha Xi class. I love reading, anything film/tv, fashion, gloomy weather, and traveling! A fun fact about me is I used to have bright pink hair. Ask me for book recommendations or about the concerts I’ve been to at recruitment :)</t>
+  </si>
+  <si>
+    <t>BCEC, Marketing Association</t>
+  </si>
+  <si>
+    <t>Marketing, Consulting, Entrepreneurship</t>
   </si>
 </sst>
 </file>
@@ -1576,10 +1576,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1904,10 +1904,10 @@
   <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B49" sqref="B49"/>
+      <selection pane="bottomRight" activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2418,13 +2418,13 @@
         <v>44949.67291666667</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>453</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>454</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>455</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>415</v>
@@ -2440,7 +2440,7 @@
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="3" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>422</v>
@@ -2452,13 +2452,13 @@
         <v>56</v>
       </c>
       <c r="N11" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="P11" s="4" t="s">
         <v>457</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>458</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
@@ -2750,13 +2750,13 @@
         <v>44949.67291666667</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>477</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>478</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>479</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>415</v>
@@ -2765,32 +2765,32 @@
         <v>17</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="L18" s="4" t="s">
         <v>482</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>483</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>484</v>
       </c>
       <c r="M18" s="3" t="s">
         <v>25</v>
       </c>
       <c r="N18" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="P18" s="4" t="s">
         <v>485</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="P18" s="4" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
@@ -3088,13 +3088,13 @@
         <v>44949.67291666667</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>441</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>443</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>415</v>
@@ -3103,34 +3103,34 @@
         <v>17</v>
       </c>
       <c r="G25" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="J25" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="K25" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="L25" s="4" t="s">
         <v>447</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>448</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>449</v>
       </c>
       <c r="M25" s="4" t="s">
         <v>44</v>
       </c>
       <c r="N25" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="P25" s="4" t="s">
         <v>450</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="P25" s="4" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3186,13 +3186,13 @@
         <v>44949.67291666667</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>488</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>489</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>490</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>415</v>
@@ -3201,7 +3201,7 @@
         <v>39</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>23</v>
@@ -3210,25 +3210,25 @@
         <v>64</v>
       </c>
       <c r="J27" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="L27" s="3" t="s">
         <v>492</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>493</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>494</v>
       </c>
       <c r="M27" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3478,13 +3478,13 @@
         <v>44949.67291666667</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>460</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>462</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>415</v>
@@ -3493,7 +3493,7 @@
         <v>17</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>34</v>
@@ -3508,19 +3508,19 @@
         <v>30</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="M33" s="3" t="s">
         <v>48</v>
       </c>
       <c r="N33" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="O33" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="P33" s="4" t="s">
         <v>465</v>
-      </c>
-      <c r="O33" s="8" t="s">
-        <v>466</v>
-      </c>
-      <c r="P33" s="4" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3724,13 +3724,13 @@
         <v>44949.67291666667</v>
       </c>
       <c r="B38" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>468</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>469</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>470</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>415</v>
@@ -3739,32 +3739,32 @@
         <v>39</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>34</v>
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="3" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="K38" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="M38" s="3" t="s">
         <v>66</v>
       </c>
       <c r="N38" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="P38" s="4" t="s">
         <v>474</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="P38" s="4" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3990,25 +3990,25 @@
       </c>
       <c r="I43" s="4"/>
       <c r="J43" s="3" t="s">
-        <v>436</v>
+        <v>496</v>
       </c>
       <c r="K43" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>437</v>
+        <v>495</v>
       </c>
       <c r="M43" s="4" t="s">
         <v>31</v>
       </c>
       <c r="N43" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="O43" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="P43" s="4" t="s">
         <v>438</v>
-      </c>
-      <c r="O43" s="8" t="s">
-        <v>439</v>
-      </c>
-      <c r="P43" s="4" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed Full-Time 2022 Positions, and missing bros.
</commit_message>
<xml_diff>
--- a/src/data/summer21/bios_summer21.xlsx
+++ b/src/data/summer21/bios_summer21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\kcow\code\dspuci-website-gatsby\src\data\summer21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF187C7-E47D-4BEE-9C11-F78986EB3F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BB22E2-D6C4-40F2-B076-972C7EA01DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="1935" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5235" yWindow="2280" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="507">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1512,13 +1512,43 @@
   </si>
   <si>
     <t>Marketing, Consulting, Entrepreneurship</t>
+  </si>
+  <si>
+    <t>Jorina</t>
+  </si>
+  <si>
+    <t>jorina_chen</t>
+  </si>
+  <si>
+    <t>San Jose, CA</t>
+  </si>
+  <si>
+    <t>Innovation and Entrepreneurship</t>
+  </si>
+  <si>
+    <t>UX Design, UX Research</t>
+  </si>
+  <si>
+    <t>UX Research Intern at Zendesk</t>
+  </si>
+  <si>
+    <t>Design at UCI, STAR Group Research Assistant, WICS</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/jorinachen</t>
+  </si>
+  <si>
+    <t>jorinachen@ucidsp.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello! My name is Jorina Chen and I initiated in the spring quarter of my sophomore year with the Alpha Nu class. During my free time, I am exploring new places around Irvine or getting food with friends. Ask me about design, food, or my music taste at recruitment! </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1547,6 +1577,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1569,7 +1605,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1583,6 +1619,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1901,13 +1939,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J43" sqref="J43"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2267,448 +2305,449 @@
         <v>373</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="9" t="s">
+        <v>497</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>499</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>500</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>502</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>503</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>504</v>
+      </c>
+      <c r="O8" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J9" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L9" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P9" s="4" t="s">
         <v>333</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>44404.653217592589</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
+        <v>44404.653217592589</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
         <v>44397.382604166669</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K11" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L11" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="M11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="P11" s="4" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
         <v>44949.67291666667</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="3" t="s">
+      <c r="I12" s="4"/>
+      <c r="J12" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="K12" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="L12" s="3" t="s">
         <v>418</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="M12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="N12" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="O11" s="8" t="s">
+      <c r="O12" s="8" t="s">
         <v>456</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="P12" s="4" t="s">
         <v>457</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="P12" s="4" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>236</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
-        <v>44396.99622685185</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>126</v>
+        <v>64</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>127</v>
+        <v>245</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>128</v>
+        <v>246</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>129</v>
+        <v>247</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N14" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>131</v>
+        <v>44</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>248</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
-        <v>44397.802523148152</v>
+        <v>44396.99622685185</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>227</v>
+        <v>123</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>228</v>
+        <v>124</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>90</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="4"/>
+      <c r="I15" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J15" s="4" t="s">
-        <v>229</v>
+        <v>127</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>232</v>
+        <v>128</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>230</v>
+        <v>130</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>231</v>
+        <v>131</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>312</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
+      <c r="A16" s="5">
+        <v>44397.802523148152</v>
+      </c>
       <c r="B16" s="4" t="s">
-        <v>267</v>
+        <v>227</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>268</v>
+        <v>21</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>269</v>
+        <v>228</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>236</v>
+        <v>90</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>270</v>
+        <v>45</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>23</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4" t="s">
-        <v>271</v>
+        <v>229</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>30</v>
+        <v>232</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>272</v>
+        <v>56</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>273</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>236</v>
@@ -2717,922 +2756,918 @@
         <v>17</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>23</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>30</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>261</v>
+        <v>30</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>255</v>
+        <v>272</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>44949.67291666667</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>475</v>
+        <v>273</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>250</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>476</v>
+        <v>251</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>477</v>
+        <v>252</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>415</v>
+        <v>236</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>44949.67291666667</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>479</v>
       </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="3" t="s">
+      <c r="I19" s="4"/>
+      <c r="J19" s="3" t="s">
         <v>480</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="K19" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="L19" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="M18" s="3" t="s">
+      <c r="M19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N18" s="4" t="s">
+      <c r="N19" s="4" t="s">
         <v>483</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="O19" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="P18" s="4" t="s">
+      <c r="P19" s="4" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
+    <row r="20" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
         <v>44398.992349537039</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I20" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J20" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K20" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="L20" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="M20" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="N19" s="6" t="s">
+      <c r="N20" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="O19" s="4" t="s">
+      <c r="O20" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="P19" s="4" t="s">
+      <c r="P20" s="4" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="P20" s="4" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
-        <v>343</v>
+        <v>233</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>344</v>
+        <v>234</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>345</v>
+        <v>235</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>317</v>
+        <v>236</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>346</v>
+        <v>237</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>348</v>
+        <v>238</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>349</v>
+        <v>64</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>30</v>
+        <v>239</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>305</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>351</v>
+        <v>306</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>352</v>
+        <v>44</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>285</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>353</v>
+        <v>241</v>
       </c>
       <c r="P21" s="4" t="s">
-        <v>354</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>260</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>386</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>387</v>
-      </c>
-      <c r="M22" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="P22" s="4" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="5">
-        <v>44404.807638888888</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>23</v>
       </c>
       <c r="I23" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>44404.807638888888</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J24" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K24" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="L24" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="M24" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="N23" s="6" t="s">
+      <c r="N24" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="O23" s="6" t="s">
+      <c r="O24" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="P23" s="4" t="s">
+      <c r="P24" s="4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4" t="s">
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>236</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="M24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="N24" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="P24" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5">
-        <v>44949.67291666667</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>440</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>415</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>442</v>
+      <c r="G25" s="4" t="s">
+        <v>277</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>443</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>446</v>
+        <v>34</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>310</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>447</v>
+        <v>311</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>448</v>
+        <v>290</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>449</v>
+        <v>279</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>450</v>
+        <v>278</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>264</v>
+      <c r="A26" s="5">
+        <v>44949.67291666667</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>440</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>265</v>
+        <v>441</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>236</v>
+        <v>415</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="P26" s="4" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I27" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J27" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="K27" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="L26" s="4" t="s">
+      <c r="L27" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="M26" s="4" t="s">
+      <c r="M27" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N26" s="4" t="s">
+      <c r="N27" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="O26" s="1" t="s">
+      <c r="O27" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="P26" s="4" t="s">
+      <c r="P27" s="4" t="s">
         <v>404</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="5">
-        <v>44949.67291666667</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>486</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>487</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>415</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>489</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="M27" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N27" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="P27" s="4" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
-        <v>44409.75885416667</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>26</v>
+        <v>44949.67291666667</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>486</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>27</v>
+        <v>487</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>103</v>
+        <v>488</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>16</v>
+        <v>415</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H28" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="M28" s="4" t="s">
+      <c r="I28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="M28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N28" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="O28" s="6" t="s">
-        <v>80</v>
+      <c r="N28" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>493</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>105</v>
+        <v>494</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
-        <v>44949.67291666667</v>
+        <v>44409.75885416667</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>133</v>
+        <v>26</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>413</v>
+        <v>27</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>414</v>
+        <v>103</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>415</v>
+        <v>16</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>416</v>
+        <v>22</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>238</v>
+        <v>28</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="I29" s="4"/>
-      <c r="J29" s="3" t="s">
-        <v>91</v>
+      <c r="J29" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>418</v>
+        <v>382</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N29" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>420</v>
+        <v>31</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>421</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
-        <v>44396.99490740741</v>
+        <v>44949.67291666667</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>107</v>
+        <v>413</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>108</v>
+        <v>414</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>90</v>
+        <v>415</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>39</v>
+        <v>416</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>302</v>
+        <v>417</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="I30" s="4"/>
+      <c r="J30" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="L30" s="4" t="s">
-        <v>109</v>
+        <v>30</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>418</v>
       </c>
       <c r="M30" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N30" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="O30" s="4" t="s">
-        <v>111</v>
+      <c r="N30" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>420</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>112</v>
+        <v>421</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
+      <c r="A31" s="5">
+        <v>44396.99490740741</v>
+      </c>
       <c r="B31" s="4" t="s">
-        <v>280</v>
+        <v>106</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>281</v>
+        <v>107</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>282</v>
+        <v>108</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>236</v>
+        <v>90</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>39</v>
       </c>
       <c r="G31" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="O31" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="P31" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G32" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="H32" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4" t="s">
+      <c r="I32" s="4"/>
+      <c r="J32" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="K32" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="L31" s="4" t="s">
+      <c r="L32" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="M31" s="4" t="s">
+      <c r="M32" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="N31" s="4" t="s">
+      <c r="N32" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="O32" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="P31" s="4" t="s">
+      <c r="P32" s="4" t="s">
         <v>393</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="5">
-        <v>44411.590104166666</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="L32" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="M32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N32" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="O32" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="P32" s="4" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
-        <v>44949.67291666667</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>458</v>
+        <v>44411.590104166666</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>459</v>
+        <v>15</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>460</v>
+        <v>97</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>415</v>
+        <v>16</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>30</v>
+        <v>98</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>462</v>
-      </c>
-      <c r="M33" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="N33" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="O33" s="8" t="s">
-        <v>464</v>
+        <v>101</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="P33" s="4" t="s">
-        <v>465</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
-        <v>44409.99291666667</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>141</v>
+        <v>44949.67291666667</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>458</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>142</v>
+        <v>459</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>143</v>
+        <v>460</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>113</v>
+        <v>415</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H34" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="H34" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="K34" s="4" t="s">
-        <v>309</v>
+      <c r="I34" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M34" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="N34" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="O34" s="4" t="s">
-        <v>145</v>
+        <v>462</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="O34" s="8" t="s">
+        <v>464</v>
       </c>
       <c r="P34" s="4" t="s">
-        <v>308</v>
+        <v>465</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
-        <v>44397.626064814816</v>
+        <v>44409.99291666667</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>72</v>
+        <v>141</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>212</v>
+        <v>143</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>213</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="I35" s="4"/>
       <c r="J35" s="4" t="s">
-        <v>55</v>
+        <v>222</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>389</v>
+        <v>309</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>390</v>
+        <v>30</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="N35" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="O35" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="P35" s="3" t="s">
-        <v>214</v>
+        <v>144</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="P35" s="4" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
-        <v>44411.616377314815</v>
+        <v>44397.626064814816</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>146</v>
+        <v>212</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>16</v>
@@ -3641,48 +3676,48 @@
         <v>22</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>23</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>53</v>
+        <v>213</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>147</v>
+        <v>55</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>148</v>
+        <v>389</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>303</v>
+        <v>390</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="O36" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="P36" s="4" t="s">
-        <v>304</v>
+        <v>82</v>
+      </c>
+      <c r="P36" s="3" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
-        <v>44413.04755787037</v>
+        <v>44411.616377314815</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>200</v>
+        <v>146</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>16</v>
@@ -3691,608 +3726,660 @@
         <v>22</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I37" s="4"/>
+      <c r="I37" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="J37" s="4" t="s">
-        <v>201</v>
+        <v>147</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>202</v>
+        <v>148</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>203</v>
+        <v>303</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="O37" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P37" s="4" t="s">
-        <v>204</v>
+        <v>304</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
+        <v>44413.04755787037</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N38" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="O38" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="P38" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
         <v>44949.67291666667</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>466</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>467</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>468</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E39" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F39" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G39" s="3" t="s">
         <v>469</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H39" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I38" s="4"/>
-      <c r="J38" s="3" t="s">
+      <c r="I39" s="4"/>
+      <c r="J39" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="K38" s="3" t="s">
+      <c r="K39" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L38" s="3" t="s">
+      <c r="L39" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="M38" s="3" t="s">
+      <c r="M39" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="N38" s="4" t="s">
+      <c r="N39" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="O38" s="1" t="s">
+      <c r="O39" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="P38" s="4" t="s">
+      <c r="P39" s="4" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="5">
+    <row r="40" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
         <v>44404.80846064815</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>216</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="L39" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="M39" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N39" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="O39" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="P39" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4" t="s">
-        <v>318</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>217</v>
       </c>
       <c r="D40" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N40" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="P40" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E41" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F41" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="G41" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="K40" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="L40" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M40" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="N40" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="P40" s="4" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="5">
-        <v>44396.959282407406</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>196</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I41" s="4"/>
+      <c r="I41" s="4" t="s">
+        <v>320</v>
+      </c>
       <c r="J41" s="4" t="s">
-        <v>24</v>
+        <v>321</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>197</v>
+        <v>322</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>198</v>
+        <v>30</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N41" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="O41" s="6" t="s">
-        <v>85</v>
+        <v>46</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="P41" s="4" t="s">
-        <v>199</v>
+        <v>323</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
-        <v>44410.840196759258</v>
+        <v>44396.959282407406</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>89</v>
+        <v>195</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>28</v>
+        <v>196</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>215</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="I42" s="4"/>
       <c r="J42" s="4" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>92</v>
+        <v>197</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>93</v>
+        <v>198</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="N42" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="O42" s="4" t="s">
-        <v>95</v>
+        <v>70</v>
+      </c>
+      <c r="O42" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="P42" s="4" t="s">
-        <v>96</v>
+        <v>199</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
-        <v>44949.67291666667</v>
+        <v>44410.840196759258</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>432</v>
+        <v>87</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>433</v>
+        <v>88</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>434</v>
+        <v>89</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>415</v>
+        <v>90</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="H43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H43" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I43" s="4"/>
-      <c r="J43" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L43" s="3" t="s">
-        <v>495</v>
+      <c r="I43" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="L43" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N43" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="O43" s="8" t="s">
-        <v>437</v>
+        <v>66</v>
+      </c>
+      <c r="N43" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="P43" s="4" t="s">
-        <v>438</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
-        <v>44397.036516203705</v>
+        <v>44949.67291666667</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>116</v>
+        <v>432</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>117</v>
+        <v>433</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>118</v>
+        <v>434</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>90</v>
+        <v>415</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G44" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>42</v>
+      <c r="G44" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="I44" s="4"/>
-      <c r="J44" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>385</v>
-      </c>
-      <c r="L44" s="4" t="s">
-        <v>40</v>
+      <c r="J44" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>495</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N44" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="O44" s="4" t="s">
-        <v>121</v>
+        <v>31</v>
+      </c>
+      <c r="N44" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="O44" s="8" t="s">
+        <v>437</v>
       </c>
       <c r="P44" s="4" t="s">
-        <v>122</v>
+        <v>438</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
-        <v>44411.776064814818</v>
+        <v>44397.036516203705</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>149</v>
+        <v>116</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>150</v>
+        <v>117</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>39</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="I45" s="4"/>
       <c r="J45" s="4" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="L45" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>115</v>
+        <v>25</v>
       </c>
       <c r="N45" s="6" t="s">
-        <v>153</v>
+        <v>120</v>
       </c>
       <c r="O45" s="4" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="P45" s="4" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="4"/>
+      <c r="A46" s="5">
+        <v>44411.776064814818</v>
+      </c>
       <c r="B46" s="4" t="s">
-        <v>374</v>
+        <v>149</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>150</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>375</v>
+        <v>151</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>317</v>
+        <v>113</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>39</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>376</v>
+        <v>152</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>320</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="I46" s="4"/>
       <c r="J46" s="4" t="s">
-        <v>409</v>
+        <v>55</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>408</v>
+        <v>391</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>378</v>
+        <v>40</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N46" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="O46" s="1" t="s">
-        <v>380</v>
+        <v>115</v>
+      </c>
+      <c r="N46" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="O46" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="P46" s="4" t="s">
-        <v>381</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="5">
-        <v>44405.648368055554</v>
-      </c>
+      <c r="A47" s="4"/>
       <c r="B47" s="4" t="s">
-        <v>183</v>
+        <v>374</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>185</v>
+        <v>375</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>90</v>
+        <v>317</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>39</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>186</v>
+        <v>376</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>34</v>
+        <v>377</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>126</v>
+        <v>320</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>187</v>
+        <v>409</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>188</v>
+        <v>408</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>189</v>
+        <v>378</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="N47" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="O47" s="4" t="s">
-        <v>191</v>
+        <v>35</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>380</v>
       </c>
       <c r="P47" s="4" t="s">
-        <v>192</v>
+        <v>381</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
-        <v>44396.946180555555</v>
+        <v>44405.648368055554</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>156</v>
+        <v>183</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>90</v>
       </c>
       <c r="F48" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N48" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="O48" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="P48" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="5">
+        <v>44396.946180555555</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F49" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="G49" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H48" s="4" t="s">
+      <c r="H49" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4" t="s">
+      <c r="I49" s="4"/>
+      <c r="J49" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="K48" s="4" t="s">
+      <c r="K49" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="L48" s="4" t="s">
+      <c r="L49" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="M48" s="4" t="s">
+      <c r="M49" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N48" s="6" t="s">
+      <c r="N49" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="O48" s="4" t="s">
+      <c r="O49" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="P48" s="4" t="s">
+      <c r="P49" s="4" t="s">
         <v>163</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P48">
-    <sortCondition ref="C2:C48"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P49">
+    <sortCondition ref="C2:C49"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="O20" r:id="rId1" xr:uid="{9E307C65-887C-5044-8DB8-E71EB3F10045}"/>
-    <hyperlink ref="O13" r:id="rId2" xr:uid="{4A81FE9A-EBAB-0747-B2F3-61D7490B1D68}"/>
-    <hyperlink ref="O22" r:id="rId3" xr:uid="{85DCA030-31D8-4740-B777-FBA97285460E}"/>
-    <hyperlink ref="O26" r:id="rId4" xr:uid="{5A40EFE8-502D-2149-ACBE-311EA5579DF3}"/>
-    <hyperlink ref="O16" r:id="rId5" xr:uid="{7E0B92DD-CBCC-8F46-B940-A199BDE9BF18}"/>
-    <hyperlink ref="O24" r:id="rId6" xr:uid="{6A6E0364-629D-FF44-817A-6C9F4E3C32C0}"/>
-    <hyperlink ref="O31" r:id="rId7" xr:uid="{7DAAB33D-9347-8F48-A5B6-88CA9022F3F4}"/>
-    <hyperlink ref="N10" r:id="rId8" xr:uid="{3FEE33F3-63FD-49C4-92AB-1042A2591AA6}"/>
-    <hyperlink ref="O10" r:id="rId9" xr:uid="{7CBE67B6-B9B5-45EE-9470-F4AA5E5FF358}"/>
-    <hyperlink ref="N40" r:id="rId10" xr:uid="{56DE9EB8-7714-4395-9CD4-AF9B7F618754}"/>
-    <hyperlink ref="O40" r:id="rId11" xr:uid="{C79E0D61-6BF8-4D23-9016-8FA43E7BA486}"/>
-    <hyperlink ref="N8" r:id="rId12" xr:uid="{5B38EE64-6D4D-430D-9621-00ED2C8B8D7A}"/>
-    <hyperlink ref="O8" r:id="rId13" xr:uid="{01DBDDE2-32E1-4266-A6A7-FDED7088E189}"/>
+    <hyperlink ref="O21" r:id="rId1" xr:uid="{9E307C65-887C-5044-8DB8-E71EB3F10045}"/>
+    <hyperlink ref="O14" r:id="rId2" xr:uid="{4A81FE9A-EBAB-0747-B2F3-61D7490B1D68}"/>
+    <hyperlink ref="O23" r:id="rId3" xr:uid="{85DCA030-31D8-4740-B777-FBA97285460E}"/>
+    <hyperlink ref="O27" r:id="rId4" xr:uid="{5A40EFE8-502D-2149-ACBE-311EA5579DF3}"/>
+    <hyperlink ref="O17" r:id="rId5" xr:uid="{7E0B92DD-CBCC-8F46-B940-A199BDE9BF18}"/>
+    <hyperlink ref="O25" r:id="rId6" xr:uid="{6A6E0364-629D-FF44-817A-6C9F4E3C32C0}"/>
+    <hyperlink ref="O32" r:id="rId7" xr:uid="{7DAAB33D-9347-8F48-A5B6-88CA9022F3F4}"/>
+    <hyperlink ref="N11" r:id="rId8" xr:uid="{3FEE33F3-63FD-49C4-92AB-1042A2591AA6}"/>
+    <hyperlink ref="O11" r:id="rId9" xr:uid="{7CBE67B6-B9B5-45EE-9470-F4AA5E5FF358}"/>
+    <hyperlink ref="N41" r:id="rId10" xr:uid="{56DE9EB8-7714-4395-9CD4-AF9B7F618754}"/>
+    <hyperlink ref="O41" r:id="rId11" xr:uid="{C79E0D61-6BF8-4D23-9016-8FA43E7BA486}"/>
+    <hyperlink ref="N9" r:id="rId12" xr:uid="{5B38EE64-6D4D-430D-9621-00ED2C8B8D7A}"/>
+    <hyperlink ref="O9" r:id="rId13" xr:uid="{01DBDDE2-32E1-4266-A6A7-FDED7088E189}"/>
     <hyperlink ref="N3" r:id="rId14" xr:uid="{D7196034-9BFC-401F-8AD8-444A5A8F0488}"/>
     <hyperlink ref="O3" r:id="rId15" xr:uid="{EBB06DFB-D7BE-4833-AFA8-B29F5EB78FCE}"/>
-    <hyperlink ref="N21" r:id="rId16" xr:uid="{75085428-AD2A-4222-ACFA-ED2B329717F2}"/>
-    <hyperlink ref="O21" r:id="rId17" xr:uid="{8AD637F9-AD2E-42B3-9D8D-76C11471058D}"/>
-    <hyperlink ref="N12" r:id="rId18" xr:uid="{120B96FF-057F-4C8A-B466-35389F9A4CD8}"/>
-    <hyperlink ref="O12" r:id="rId19" xr:uid="{BC0B539C-D47A-4142-91C2-D1991320DA6E}"/>
+    <hyperlink ref="N22" r:id="rId16" xr:uid="{75085428-AD2A-4222-ACFA-ED2B329717F2}"/>
+    <hyperlink ref="O22" r:id="rId17" xr:uid="{8AD637F9-AD2E-42B3-9D8D-76C11471058D}"/>
+    <hyperlink ref="N13" r:id="rId18" xr:uid="{120B96FF-057F-4C8A-B466-35389F9A4CD8}"/>
+    <hyperlink ref="O13" r:id="rId19" xr:uid="{BC0B539C-D47A-4142-91C2-D1991320DA6E}"/>
     <hyperlink ref="N7" r:id="rId20" xr:uid="{B153E7EE-184D-4F41-8EAC-022CA1AFC245}"/>
     <hyperlink ref="O7" r:id="rId21" xr:uid="{53635958-96CA-44CA-B081-1F20CB88B225}"/>
-    <hyperlink ref="N46" r:id="rId22" xr:uid="{BC598059-63C8-462E-852A-A0B1E342929A}"/>
-    <hyperlink ref="O46" r:id="rId23" xr:uid="{31B14771-D13B-4480-85D7-DFC9490D3475}"/>
-    <hyperlink ref="O29" r:id="rId24" xr:uid="{FD117BD8-3AF2-4B01-B279-EDBCF98F0DDE}"/>
+    <hyperlink ref="N47" r:id="rId22" xr:uid="{BC598059-63C8-462E-852A-A0B1E342929A}"/>
+    <hyperlink ref="O47" r:id="rId23" xr:uid="{31B14771-D13B-4480-85D7-DFC9490D3475}"/>
+    <hyperlink ref="O30" r:id="rId24" xr:uid="{FD117BD8-3AF2-4B01-B279-EDBCF98F0DDE}"/>
     <hyperlink ref="O6" r:id="rId25" xr:uid="{64F20DE1-847E-4E86-803E-F389D93019A9}"/>
-    <hyperlink ref="O43" r:id="rId26" xr:uid="{7DB90521-7C8C-4C1A-8730-FA86718C5AF0}"/>
-    <hyperlink ref="O25" r:id="rId27" xr:uid="{51103739-3C3F-4649-A2A9-86769340C288}"/>
-    <hyperlink ref="O11" r:id="rId28" xr:uid="{B1F33C14-8637-4F79-A182-6EE9FEF1EA1B}"/>
-    <hyperlink ref="O33" r:id="rId29" xr:uid="{66D8CBF6-5E57-4F61-A1EC-FCB9108C690A}"/>
-    <hyperlink ref="O18" r:id="rId30" xr:uid="{E247FEE5-2EDF-46BC-9378-1037D3ADE7CB}"/>
-    <hyperlink ref="O27" r:id="rId31" xr:uid="{508AB42F-5DE3-4501-AEE5-8A5419C86EFF}"/>
-    <hyperlink ref="O17" r:id="rId32" xr:uid="{448DA057-37C3-3B4D-9D30-C27C2FD902D3}"/>
-    <hyperlink ref="O38" r:id="rId33" xr:uid="{825A5283-6544-4A21-BDF3-5938EB858390}"/>
+    <hyperlink ref="O44" r:id="rId26" xr:uid="{7DB90521-7C8C-4C1A-8730-FA86718C5AF0}"/>
+    <hyperlink ref="O26" r:id="rId27" xr:uid="{51103739-3C3F-4649-A2A9-86769340C288}"/>
+    <hyperlink ref="O12" r:id="rId28" xr:uid="{B1F33C14-8637-4F79-A182-6EE9FEF1EA1B}"/>
+    <hyperlink ref="O34" r:id="rId29" xr:uid="{66D8CBF6-5E57-4F61-A1EC-FCB9108C690A}"/>
+    <hyperlink ref="O19" r:id="rId30" xr:uid="{E247FEE5-2EDF-46BC-9378-1037D3ADE7CB}"/>
+    <hyperlink ref="O28" r:id="rId31" xr:uid="{508AB42F-5DE3-4501-AEE5-8A5419C86EFF}"/>
+    <hyperlink ref="O18" r:id="rId32" xr:uid="{448DA057-37C3-3B4D-9D30-C27C2FD902D3}"/>
+    <hyperlink ref="O39" r:id="rId33" xr:uid="{825A5283-6544-4A21-BDF3-5938EB858390}"/>
+    <hyperlink ref="N8" r:id="rId34" xr:uid="{9A1CEE31-0154-4921-8820-F8D298A7C07E}"/>
+    <hyperlink ref="O8" r:id="rId35" xr:uid="{7649E44C-469A-4A42-AA4D-A7B9E1151C0A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId34"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId36"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated President's Image and name, as well as SVP number
</commit_message>
<xml_diff>
--- a/src/data/summer21/bios_summer21.xlsx
+++ b/src/data/summer21/bios_summer21.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\kcow\code\dspuci-website-gatsby\src\data\winter23\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\kcow\code\dspuci-website-gatsby\src\data\summer21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A25C18-B248-43F4-B9C7-882CB0286D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F64BD6-8BF8-48A4-8693-B3128DFFCCD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2490" yWindow="690" windowWidth="25680" windowHeight="14910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1634,7 +1634,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1663,6 +1663,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1984,10 +1985,10 @@
   <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K39" sqref="K39"/>
+      <selection pane="bottomRight" activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2059,7 +2060,7 @@
     </row>
     <row r="2" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
-        <v>44404.516250000001</v>
+        <v>44404.515972222223</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>131</v>
@@ -2154,7 +2155,7 @@
     </row>
     <row r="4" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <v>44409.634976851848</v>
+        <v>44409.634722222225</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>62</v>
@@ -2204,7 +2205,7 @@
     </row>
     <row r="5" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>44404.857893518521</v>
+        <v>44404.857638888891</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>170</v>
@@ -2252,107 +2253,105 @@
     </row>
     <row r="6" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>295</v>
+        <v>389</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>296</v>
+        <v>171</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>297</v>
+        <v>393</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>298</v>
+        <v>382</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>40</v>
+        <v>383</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>18</v>
+        <v>397</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>469</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>301</v>
+        <v>396</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>479</v>
+        <v>395</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>302</v>
+        <v>394</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>299</v>
+        <v>392</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>300</v>
+        <v>391</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>303</v>
+        <v>390</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>342</v>
+        <v>295</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>296</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>343</v>
+        <v>297</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>298</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>344</v>
+        <v>18</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>227</v>
+        <v>50</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>345</v>
+        <v>469</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>346</v>
+        <v>301</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>347</v>
+        <v>302</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>348</v>
+        <v>299</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>349</v>
+        <v>300</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>350</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>311</v>
+        <v>342</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>313</v>
+        <v>343</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>298</v>
@@ -2361,474 +2360,474 @@
         <v>17</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="M8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N8" s="7" t="s">
+      <c r="N9" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="O9" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="P9" s="2" t="s">
         <v>318</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>44404.653217592589</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
-        <v>44397.382604166669</v>
+        <v>44404.652777777781</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="18">
+        <v>44397.381944444445</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E11" t="s">
         <v>225</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="E11" t="s">
-        <v>298</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>336</v>
+        <v>210</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="I11" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>464</v>
+      </c>
       <c r="J11" s="2" t="s">
-        <v>337</v>
+        <v>294</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>31</v>
+        <v>482</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>338</v>
+        <v>465</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>339</v>
+        <v>282</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>340</v>
+        <v>283</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>341</v>
+        <v>360</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>231</v>
+        <v>418</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>232</v>
+        <v>419</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>233</v>
+        <v>420</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>225</v>
+        <v>382</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>23</v>
+        <v>383</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>65</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>234</v>
+        <v>422</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>483</v>
+        <v>423</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>235</v>
+        <v>385</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="N12" t="s">
-        <v>275</v>
+        <v>426</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>236</v>
+        <v>425</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>237</v>
+        <v>424</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>44396.99622685185</v>
-      </c>
+      <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
-        <v>122</v>
+        <v>333</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>22</v>
+        <v>334</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>123</v>
+        <v>335</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>91</v>
+        <v>298</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>124</v>
+        <v>336</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>125</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
-        <v>126</v>
+        <v>337</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>484</v>
+        <v>31</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>127</v>
+        <v>338</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>128</v>
+        <v>339</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>129</v>
+        <v>340</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>130</v>
+        <v>341</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>44397.802523148152</v>
-      </c>
+      <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
+        <v>44396.995833333334</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>225</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>256</v>
+        <v>124</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="I15" t="s">
+        <v>125</v>
+      </c>
       <c r="J15" s="2" t="s">
-        <v>257</v>
+        <v>126</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>31</v>
+        <v>484</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="N15" t="s">
-        <v>274</v>
+        <v>128</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>258</v>
+        <v>129</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
+        <v>44397.802083333336</v>
+      </c>
       <c r="B16" s="2" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>239</v>
+        <v>22</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>240</v>
+        <v>218</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>225</v>
+        <v>91</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>241</v>
+        <v>46</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="12" t="s">
-        <v>470</v>
-      </c>
+      <c r="I16" s="12"/>
       <c r="J16" s="2" t="s">
-        <v>471</v>
+        <v>219</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>472</v>
+        <v>41</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="N16" t="s">
-        <v>273</v>
+        <v>220</v>
       </c>
       <c r="O16" s="7" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>243</v>
+        <v>293</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
-        <v>44398.992349537039</v>
-      </c>
+      <c r="A17" s="3"/>
       <c r="B17" s="2" t="s">
-        <v>164</v>
+        <v>253</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>165</v>
+        <v>254</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>166</v>
+        <v>255</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>112</v>
+        <v>225</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>68</v>
+        <v>256</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>367</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>30</v>
+        <v>257</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>487</v>
+        <v>31</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>368</v>
+        <v>31</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>114</v>
+        <v>20</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>167</v>
+        <v>274</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>168</v>
+        <v>258</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>169</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>225</v>
@@ -2837,233 +2836,235 @@
         <v>17</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>227</v>
+        <v>24</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>65</v>
+        <v>470</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>228</v>
+        <v>471</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>289</v>
+        <v>472</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="N18" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>324</v>
+        <v>444</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>325</v>
+        <v>445</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>326</v>
+        <v>446</v>
       </c>
       <c r="E19" t="s">
-        <v>298</v>
+        <v>382</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>327</v>
+        <v>447</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>330</v>
-      </c>
+        <v>448</v>
+      </c>
+      <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
-        <v>466</v>
+        <v>449</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>31</v>
+        <v>450</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>331</v>
+        <v>454</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>332</v>
+        <v>453</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="18">
+        <v>44398.991666666669</v>
+      </c>
       <c r="B20" s="2" t="s">
-        <v>244</v>
+        <v>164</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>245</v>
+        <v>165</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>246</v>
+        <v>166</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="N20" t="s">
+        <v>167</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N20" t="s">
-        <v>272</v>
-      </c>
-      <c r="O20" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
-        <v>44404.807638888888</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="G21" s="2" t="s">
-        <v>60</v>
+        <v>226</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>24</v>
+        <v>227</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>65</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>30</v>
+        <v>228</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>162</v>
+        <v>289</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>61</v>
+        <v>271</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>80</v>
+        <v>230</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>163</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
-        <v>260</v>
+        <v>324</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>261</v>
+        <v>325</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>262</v>
+        <v>326</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>225</v>
+        <v>298</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>263</v>
+        <v>327</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>35</v>
+        <v>329</v>
+      </c>
+      <c r="I22" t="s">
+        <v>330</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>135</v>
+        <v>466</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>491</v>
+        <v>31</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>292</v>
+        <v>467</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="N22" t="s">
-        <v>276</v>
+        <v>331</v>
       </c>
       <c r="O22" s="7" t="s">
-        <v>265</v>
+        <v>332</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>264</v>
+        <v>468</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>225</v>
@@ -3072,48 +3073,48 @@
         <v>17</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>113</v>
+        <v>247</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>369</v>
+        <v>284</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>370</v>
+        <v>92</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="N23" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
-        <v>44409.75885416667</v>
+        <v>44404.807638888888</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>16</v>
@@ -3122,239 +3123,237 @@
         <v>23</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I24" s="2"/>
+      <c r="I24" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="J24" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>359</v>
+        <v>490</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>104</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
-        <v>44396.99490740741</v>
-      </c>
+      <c r="A25" s="3"/>
       <c r="B25" s="2" t="s">
-        <v>105</v>
+        <v>260</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>106</v>
+        <v>261</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>107</v>
+        <v>262</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>91</v>
+        <v>225</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>48</v>
+        <v>263</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>377</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="I25" s="2"/>
       <c r="J25" s="2" t="s">
-        <v>286</v>
+        <v>135</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>108</v>
+        <v>292</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>109</v>
+        <v>276</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>110</v>
+        <v>265</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>111</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>266</v>
+        <v>407</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>267</v>
+        <v>408</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>268</v>
+        <v>412</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N26" t="s">
+        <v>413</v>
+      </c>
+      <c r="O26" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="H26" s="2" t="s">
+      <c r="F27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="N26" t="s">
-        <v>278</v>
-      </c>
-      <c r="O26" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
-        <v>44411.590104166666</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="I27" s="2" t="s">
-        <v>98</v>
+        <v>369</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>99</v>
+        <v>370</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>100</v>
+        <v>371</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>21</v>
+        <v>277</v>
       </c>
       <c r="O27" s="5" t="s">
-        <v>82</v>
+        <v>252</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>101</v>
+        <v>372</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
-        <v>44409.99291666667</v>
-      </c>
+      <c r="A28" s="3"/>
       <c r="B28" s="2" t="s">
-        <v>139</v>
+        <v>455</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>140</v>
+        <v>460</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>141</v>
+        <v>461</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>112</v>
+        <v>382</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>70</v>
+        <v>462</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I28" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="J28" s="2" t="s">
-        <v>213</v>
+        <v>463</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>496</v>
+        <v>459</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>31</v>
+        <v>458</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>142</v>
+        <v>454</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>143</v>
+        <v>456</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>291</v>
+        <v>457</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
-        <v>44397.626064814816</v>
+        <v>44409.758333333331</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>203</v>
+        <v>102</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>16</v>
@@ -3363,1017 +3362,1000 @@
         <v>23</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>204</v>
-      </c>
+      <c r="I29" s="2"/>
       <c r="J29" s="2" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>497</v>
+        <v>359</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>363</v>
+        <v>103</v>
       </c>
       <c r="M29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O29" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="P29" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+      <c r="B30" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="M30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N29" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O29" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="P29" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
-        <v>44411.616377314815</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="N30" s="1" t="s">
-        <v>55</v>
+        <v>386</v>
       </c>
       <c r="O30" s="5" t="s">
-        <v>84</v>
+        <v>387</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>288</v>
+        <v>388</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
-        <v>44413.04755787037</v>
+        <v>44396.994444444441</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>192</v>
+        <v>107</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="O31" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+      <c r="B32" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="18">
+        <v>44411.589583333334</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="N31" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O31" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="P31" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
-        <v>44404.80846064815</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="M32" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N32" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="O32" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="P32" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="G33" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>306</v>
+        <v>98</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>307</v>
+        <v>99</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>309</v>
+        <v>21</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>310</v>
+        <v>82</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>308</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
-        <v>44396.959282407406</v>
-      </c>
+      <c r="A34" s="3"/>
       <c r="B34" s="2" t="s">
-        <v>69</v>
+        <v>427</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>37</v>
+        <v>428</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>188</v>
+        <v>434</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>16</v>
+        <v>382</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>189</v>
+        <v>429</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I34" s="2"/>
+      <c r="I34" s="2" t="s">
+        <v>212</v>
+      </c>
       <c r="J34" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>502</v>
+        <v>31</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>190</v>
+        <v>430</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>71</v>
+        <v>433</v>
       </c>
       <c r="O34" s="5" t="s">
-        <v>86</v>
+        <v>432</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>191</v>
+        <v>431</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
-        <v>44410.840196759258</v>
+        <v>44409.992361111108</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>88</v>
+        <v>139</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>89</v>
+        <v>140</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>90</v>
+        <v>141</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>206</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="I35" s="2"/>
       <c r="J35" s="2" t="s">
-        <v>92</v>
+        <v>213</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>67</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>94</v>
+        <v>142</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>96</v>
+        <v>291</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
-        <v>44397.036516203705</v>
+        <v>44397.625694444447</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>115</v>
+        <v>73</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>117</v>
+        <v>203</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>118</v>
+        <v>42</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I36" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>204</v>
+      </c>
       <c r="J36" s="2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>41</v>
+        <v>363</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>119</v>
+        <v>75</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="P36" s="2" t="s">
-        <v>121</v>
+        <v>83</v>
+      </c>
+      <c r="P36" s="11" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
-        <v>44411.776064814818</v>
+        <v>44411.615972222222</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>146</v>
+        <v>52</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>147</v>
+        <v>53</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>149</v>
+        <v>29</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I37" s="2"/>
+      <c r="I37" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="J37" s="2" t="s">
-        <v>56</v>
+        <v>145</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>41</v>
+        <v>287</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>114</v>
+        <v>45</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>150</v>
+        <v>55</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>151</v>
+        <v>84</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>152</v>
+        <v>288</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="18">
+        <v>44413.047222222223</v>
+      </c>
       <c r="B38" s="2" t="s">
-        <v>351</v>
+        <v>72</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>147</v>
+        <v>76</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>352</v>
+        <v>192</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>298</v>
+        <v>16</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>353</v>
+        <v>60</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>306</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="I38" s="2"/>
       <c r="J38" s="2" t="s">
-        <v>376</v>
+        <v>193</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>375</v>
+        <v>499</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>355</v>
+        <v>194</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="N38" s="7" t="s">
-        <v>356</v>
+        <v>77</v>
       </c>
       <c r="O38" s="7" t="s">
-        <v>357</v>
+        <v>85</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>358</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
-        <v>44405.648368055554</v>
-      </c>
+      <c r="A39" s="3"/>
       <c r="B39" s="2" t="s">
-        <v>177</v>
+        <v>435</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>178</v>
+        <v>436</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>179</v>
+        <v>437</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>91</v>
+        <v>382</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>180</v>
+        <v>438</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I39" s="2" t="s">
-        <v>125</v>
-      </c>
+      <c r="I39" s="2"/>
       <c r="J39" s="2" t="s">
-        <v>181</v>
+        <v>439</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>506</v>
+        <v>31</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>182</v>
+        <v>440</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>183</v>
+        <v>443</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>184</v>
+        <v>442</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>185</v>
+        <v>441</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
-        <v>44396.946180555555</v>
+        <v>44404.808333333334</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>153</v>
+        <v>207</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>154</v>
+        <v>208</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>155</v>
+        <v>209</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>38</v>
+        <v>210</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="I40" s="2"/>
+        <v>211</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>212</v>
+      </c>
       <c r="J40" s="2" t="s">
-        <v>378</v>
+        <v>213</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>379</v>
+        <v>500</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>157</v>
+        <v>290</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>158</v>
+        <v>214</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>159</v>
+        <v>215</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>131</v>
+        <v>304</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>380</v>
+        <v>208</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>381</v>
+        <v>305</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>382</v>
+        <v>298</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>383</v>
+        <v>40</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>384</v>
+        <v>48</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>227</v>
+        <v>35</v>
+      </c>
+      <c r="I41" t="s">
+        <v>306</v>
       </c>
       <c r="J41" s="12" t="s">
-        <v>92</v>
+        <v>307</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>423</v>
+        <v>501</v>
       </c>
       <c r="L41" s="12" t="s">
-        <v>385</v>
+        <v>31</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="N41" t="s">
-        <v>386</v>
+        <v>309</v>
       </c>
       <c r="O41" s="13" t="s">
-        <v>387</v>
+        <v>310</v>
       </c>
       <c r="P41" s="14" t="s">
-        <v>388</v>
+        <v>308</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="18">
+        <v>44396.959027777775</v>
+      </c>
       <c r="B42" s="14" t="s">
-        <v>389</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>171</v>
+        <v>37</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>393</v>
+        <v>188</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>382</v>
+        <v>16</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>383</v>
+        <v>23</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>397</v>
+        <v>189</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="J42" s="12" t="s">
-        <v>396</v>
+        <v>25</v>
       </c>
       <c r="K42" s="16" t="s">
-        <v>395</v>
+        <v>502</v>
       </c>
       <c r="L42" s="14" t="s">
-        <v>394</v>
+        <v>190</v>
       </c>
       <c r="M42" s="12" t="s">
         <v>26</v>
       </c>
       <c r="N42" t="s">
-        <v>392</v>
+        <v>71</v>
       </c>
       <c r="O42" s="15" t="s">
-        <v>391</v>
+        <v>86</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>390</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="18">
+        <v>44410.839583333334</v>
+      </c>
       <c r="B43" s="2" t="s">
-        <v>398</v>
+        <v>88</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>399</v>
+        <v>89</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>400</v>
+        <v>90</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>382</v>
+        <v>91</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>401</v>
+        <v>29</v>
       </c>
       <c r="H43" s="12" t="s">
         <v>24</v>
       </c>
+      <c r="I43" t="s">
+        <v>206</v>
+      </c>
       <c r="J43" s="12" t="s">
-        <v>402</v>
+        <v>92</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>31</v>
+        <v>503</v>
       </c>
       <c r="L43" s="12" t="s">
-        <v>403</v>
+        <v>93</v>
       </c>
       <c r="M43" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="N43" t="s">
-        <v>404</v>
+        <v>94</v>
       </c>
       <c r="O43" s="17" t="s">
-        <v>405</v>
+        <v>95</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="12" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>382</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>421</v>
+        <v>401</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>409</v>
-      </c>
-      <c r="I44" s="12" t="s">
-        <v>410</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="I44" s="12"/>
       <c r="J44" s="12" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>417</v>
+        <v>31</v>
       </c>
       <c r="L44" s="14" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="N44" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="O44" s="13" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="18">
+        <v>44397.036111111112</v>
+      </c>
       <c r="B45" s="14" t="s">
-        <v>418</v>
+        <v>115</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>419</v>
+        <v>116</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>420</v>
+        <v>117</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>382</v>
+        <v>91</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>383</v>
+        <v>40</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>48</v>
+        <v>118</v>
       </c>
       <c r="H45" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J45" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="K45" s="12" t="s">
+        <v>504</v>
+      </c>
+      <c r="L45" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="M45" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="N45" t="s">
+        <v>119</v>
+      </c>
+      <c r="O45" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="P45" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="18">
+        <v>44411.775694444441</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="H46" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J45" s="12" t="s">
-        <v>422</v>
-      </c>
-      <c r="K45" s="12" t="s">
-        <v>423</v>
-      </c>
-      <c r="L45" s="12" t="s">
-        <v>385</v>
-      </c>
-      <c r="M45" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="N45" t="s">
-        <v>426</v>
-      </c>
-      <c r="O45" s="17" t="s">
-        <v>425</v>
-      </c>
-      <c r="P45" s="14" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="12" t="s">
-        <v>427</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G46" s="12" t="s">
-        <v>429</v>
-      </c>
-      <c r="H46" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>212</v>
-      </c>
+      <c r="I46" s="2"/>
       <c r="J46" s="12" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>31</v>
+        <v>505</v>
       </c>
       <c r="L46" s="14" t="s">
-        <v>430</v>
+        <v>41</v>
       </c>
       <c r="M46" s="12" t="s">
-        <v>49</v>
+        <v>114</v>
       </c>
       <c r="N46" t="s">
-        <v>433</v>
+        <v>150</v>
       </c>
       <c r="O46" s="17" t="s">
-        <v>432</v>
+        <v>151</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>431</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
-        <v>435</v>
+        <v>351</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>436</v>
+        <v>147</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>437</v>
+        <v>352</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>382</v>
+        <v>298</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>438</v>
+        <v>353</v>
       </c>
       <c r="H47" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="I47" t="s">
+        <v>306</v>
+      </c>
+      <c r="J47" s="12" t="s">
+        <v>376</v>
+      </c>
+      <c r="K47" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="L47" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="M47" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N47" t="s">
+        <v>356</v>
+      </c>
+      <c r="O47" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="18">
+        <v>44405.647916666669</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="H48" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J47" s="12" t="s">
-        <v>439</v>
-      </c>
-      <c r="K47" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="L47" s="12" t="s">
-        <v>440</v>
-      </c>
-      <c r="M47" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="N47" t="s">
-        <v>443</v>
-      </c>
-      <c r="O47" s="13" t="s">
-        <v>442</v>
-      </c>
-      <c r="P47" s="2" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="12" t="s">
-        <v>444</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G48" s="12" t="s">
-        <v>447</v>
-      </c>
-      <c r="H48" s="12" t="s">
-        <v>448</v>
+      <c r="I48" t="s">
+        <v>125</v>
       </c>
       <c r="J48" s="12" t="s">
-        <v>449</v>
+        <v>181</v>
       </c>
       <c r="K48" s="12" t="s">
-        <v>450</v>
+        <v>506</v>
       </c>
       <c r="L48" s="14" t="s">
-        <v>451</v>
+        <v>182</v>
       </c>
       <c r="M48" s="12" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="N48" t="s">
-        <v>454</v>
+        <v>183</v>
       </c>
       <c r="O48" s="13" t="s">
-        <v>453</v>
+        <v>184</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="49" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="18">
+        <v>44396.945833333331</v>
+      </c>
       <c r="B49" s="12" t="s">
-        <v>455</v>
+        <v>153</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>460</v>
+        <v>154</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>461</v>
+        <v>155</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>382</v>
+        <v>91</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>462</v>
+        <v>38</v>
       </c>
       <c r="H49" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I49" s="12" t="s">
-        <v>65</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="I49" s="12"/>
       <c r="J49" s="12" t="s">
-        <v>463</v>
+        <v>378</v>
       </c>
       <c r="K49" s="12" t="s">
-        <v>459</v>
+        <v>379</v>
       </c>
       <c r="L49" s="12" t="s">
-        <v>458</v>
+        <v>157</v>
       </c>
       <c r="M49" s="12" t="s">
         <v>32</v>
       </c>
       <c r="N49" t="s">
-        <v>454</v>
+        <v>158</v>
       </c>
       <c r="O49" s="13" t="s">
-        <v>456</v>
+        <v>159</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>457</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P40">
     <sortCondition ref="C2:C40"/>
   </sortState>
-  <hyperlinks>
-    <hyperlink ref="O18" r:id="rId1" xr:uid="{9E307C65-887C-5044-8DB8-E71EB3F10045}"/>
-    <hyperlink ref="O12" r:id="rId2" xr:uid="{4A81FE9A-EBAB-0747-B2F3-61D7490B1D68}"/>
-    <hyperlink ref="O16" r:id="rId3" xr:uid="{448DA057-37C3-3B4D-9D30-C27C2FD902D3}"/>
-    <hyperlink ref="O20" r:id="rId4" xr:uid="{85DCA030-31D8-4740-B777-FBA97285460E}"/>
-    <hyperlink ref="O23" r:id="rId5" xr:uid="{5A40EFE8-502D-2149-ACBE-311EA5579DF3}"/>
-    <hyperlink ref="O15" r:id="rId6" xr:uid="{7E0B92DD-CBCC-8F46-B940-A199BDE9BF18}"/>
-    <hyperlink ref="O22" r:id="rId7" xr:uid="{6A6E0364-629D-FF44-817A-6C9F4E3C32C0}"/>
-    <hyperlink ref="O26" r:id="rId8" xr:uid="{7DAAB33D-9347-8F48-A5B6-88CA9022F3F4}"/>
-    <hyperlink ref="N10" r:id="rId9" xr:uid="{3FEE33F3-63FD-49C4-92AB-1042A2591AA6}"/>
-    <hyperlink ref="O10" r:id="rId10" xr:uid="{7CBE67B6-B9B5-45EE-9470-F4AA5E5FF358}"/>
-    <hyperlink ref="N6" r:id="rId11" xr:uid="{7712592D-C212-4A93-BA25-D4658CFA663A}"/>
-    <hyperlink ref="O6" r:id="rId12" xr:uid="{E70F50EC-A19F-4DA1-9215-7A17F732F801}"/>
-    <hyperlink ref="N33" r:id="rId13" xr:uid="{56DE9EB8-7714-4395-9CD4-AF9B7F618754}"/>
-    <hyperlink ref="O33" r:id="rId14" xr:uid="{C79E0D61-6BF8-4D23-9016-8FA43E7BA486}"/>
-    <hyperlink ref="N8" r:id="rId15" xr:uid="{5B38EE64-6D4D-430D-9621-00ED2C8B8D7A}"/>
-    <hyperlink ref="O8" r:id="rId16" xr:uid="{01DBDDE2-32E1-4266-A6A7-FDED7088E189}"/>
-    <hyperlink ref="N3" r:id="rId17" xr:uid="{D7196034-9BFC-401F-8AD8-444A5A8F0488}"/>
-    <hyperlink ref="O3" r:id="rId18" xr:uid="{EBB06DFB-D7BE-4833-AFA8-B29F5EB78FCE}"/>
-    <hyperlink ref="N19" r:id="rId19" xr:uid="{75085428-AD2A-4222-ACFA-ED2B329717F2}"/>
-    <hyperlink ref="O19" r:id="rId20" xr:uid="{8AD637F9-AD2E-42B3-9D8D-76C11471058D}"/>
-    <hyperlink ref="N11" r:id="rId21" xr:uid="{120B96FF-057F-4C8A-B466-35389F9A4CD8}"/>
-    <hyperlink ref="O11" r:id="rId22" xr:uid="{BC0B539C-D47A-4142-91C2-D1991320DA6E}"/>
-    <hyperlink ref="N7" r:id="rId23" xr:uid="{B153E7EE-184D-4F41-8EAC-022CA1AFC245}"/>
-    <hyperlink ref="O7" r:id="rId24" xr:uid="{53635958-96CA-44CA-B081-1F20CB88B225}"/>
-    <hyperlink ref="N38" r:id="rId25" xr:uid="{BC598059-63C8-462E-852A-A0B1E342929A}"/>
-    <hyperlink ref="O38" r:id="rId26" xr:uid="{31B14771-D13B-4480-85D7-DFC9490D3475}"/>
-    <hyperlink ref="O41" r:id="rId27" xr:uid="{FD117BD8-3AF2-4B01-B279-EDBCF98F0DDE}"/>
-    <hyperlink ref="O42" r:id="rId28" xr:uid="{D4A3CA04-CD4C-4338-BACB-FD95FC1D4844}"/>
-    <hyperlink ref="O43" r:id="rId29" xr:uid="{F7DE7C11-9447-465E-812A-ADFF452D4D5F}"/>
-    <hyperlink ref="O44" r:id="rId30" xr:uid="{9247102E-9B8B-4C42-93C3-183D39CC5612}"/>
-    <hyperlink ref="O45" r:id="rId31" xr:uid="{4552F4D7-9ACE-49A0-B879-F760CCA821F2}"/>
-    <hyperlink ref="O46" r:id="rId32" xr:uid="{D337D896-75C9-437F-8A98-6A815843CEB1}"/>
-    <hyperlink ref="O47" r:id="rId33" xr:uid="{07551572-0A8E-421C-B666-8652DBC5B3EA}"/>
-    <hyperlink ref="O48" r:id="rId34" xr:uid="{71B3F31B-1BE4-438D-9EB9-F1FDD66C816C}"/>
-    <hyperlink ref="O49" r:id="rId35" xr:uid="{9F5CDBFE-7EB2-412A-B6E5-CE95649DCD2E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId36"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>